<commit_message>
Added Powerpoint export from Titis worksheet
</commit_message>
<xml_diff>
--- a/MSP Reporting Tool.xlsx
+++ b/MSP Reporting Tool.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Development Areas\MSP Reporting Tool\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAC04107-2845-467C-8003-95600458CEC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150402E0-E292-48F8-A436-057F5D5418A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F7485911-4FC0-4026-A472-9F894C577CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Look Ahead Report" sheetId="129" state="hidden" r:id="rId2"/>
-    <sheet name="got" sheetId="147" r:id="rId3"/>
-    <sheet name="Togo" sheetId="148" r:id="rId4"/>
-    <sheet name="Benue" sheetId="149" r:id="rId5"/>
-    <sheet name="Migration" sheetId="150" r:id="rId6"/>
-    <sheet name="lumidee" sheetId="151" r:id="rId7"/>
+    <sheet name="got" sheetId="181" r:id="rId3"/>
+    <sheet name="Togo" sheetId="182" r:id="rId4"/>
+    <sheet name="Benue" sheetId="183" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="LA_PERIOD">Main!$T$4</definedName>
     <definedName name="LEVEL">Main!$T$5</definedName>
     <definedName name="MPP_FILEPATH">Main!$T$6</definedName>
+    <definedName name="NO_PROJS">Main!$T$3</definedName>
+    <definedName name="PROJ_IND">Main!$U$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="79">
   <si>
     <t>Business Milestones</t>
   </si>
@@ -181,69 +181,9 @@
     <t>GIT Design Start</t>
   </si>
   <si>
-    <t>GIT Build End</t>
-  </si>
-  <si>
-    <t>GIT Test Start</t>
-  </si>
-  <si>
-    <t>GIT System Test Start</t>
-  </si>
-  <si>
-    <t>GIT System Test End  (IT Readiness Assessment 3.2 A signed off)</t>
-  </si>
-  <si>
-    <t>GIT SI Test Start</t>
-  </si>
-  <si>
-    <t>GIT SI Test End  (IT Readiness Assessment 3.2 B signed off)</t>
-  </si>
-  <si>
-    <t>GIT UAT Start</t>
-  </si>
-  <si>
-    <t>GIT UAT End</t>
-  </si>
-  <si>
-    <t>GIT NFT Start</t>
-  </si>
-  <si>
-    <t>GIT NFT End</t>
-  </si>
-  <si>
-    <t>GIT OAT Start</t>
-  </si>
-  <si>
-    <t>GIT OAT End</t>
-  </si>
-  <si>
-    <t>GIT Regression Test Start</t>
-  </si>
-  <si>
-    <t>GIT Regression Test End</t>
-  </si>
-  <si>
-    <t>All SI Deliverables delivered/complete</t>
-  </si>
-  <si>
-    <t>SI Approval for Implementation to proceed (+3 days after SD Gateway 1 Approval)</t>
-  </si>
-  <si>
-    <t>GIT Test End   (IT Readiness Assessment 3.3 signed off)</t>
-  </si>
-  <si>
-    <t>GIT Develop End</t>
-  </si>
-  <si>
     <t>GIT Deploy Stage</t>
   </si>
   <si>
-    <t>GIT Live Start</t>
-  </si>
-  <si>
-    <t>GIT Live End</t>
-  </si>
-  <si>
     <t>GIT Benefits Stage</t>
   </si>
   <si>
@@ -283,12 +223,6 @@
     <t>-499-251</t>
   </si>
   <si>
-    <t>-499-292</t>
-  </si>
-  <si>
-    <t>-499-294</t>
-  </si>
-  <si>
     <t>Ref</t>
   </si>
   <si>
@@ -340,10 +274,13 @@
     <t>No Tasks</t>
   </si>
   <si>
-    <t>Migration</t>
-  </si>
-  <si>
-    <t>lumidee</t>
+    <t>No Projs</t>
+  </si>
+  <si>
+    <t>Look ahead</t>
+  </si>
+  <si>
+    <t>Path</t>
   </si>
 </sst>
 </file>
@@ -449,43 +386,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{ED3DACD9-5B4B-47B4-AB17-B329AFBAD914}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -908,254 +809,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!ShtMain.BtnLAR4wClick" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="BtnLAR4w">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711CF68E-298B-4110-AF75-6C65B51F5C08}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2647950" y="1095376"/>
-          <a:ext cx="781050" cy="323850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="DA2C38"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                  <a:prstClr val="black">
-                    <a:alpha val="50000"/>
-                  </a:prstClr>
-                </a:innerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="E8E8E8"/>
-              </a:solidFill>
-              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>4</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="E8E8E8"/>
-              </a:solidFill>
-              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Weeks</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="E8E8E8"/>
-            </a:solidFill>
-            <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!ShtMain.BtnLAR12wClick" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="BtnLAR12w">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{764C1C12-42C1-4E22-9956-6BC2FBCAE756}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2647950" y="771526"/>
-          <a:ext cx="781050" cy="323850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="DA2C38"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="DA2C38"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-            <a:prstClr val="black">
-              <a:alpha val="50000"/>
-            </a:prstClr>
-          </a:innerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="756A6D"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="E8E8E8"/>
-              </a:solidFill>
-              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>12</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="E8E8E8"/>
-              </a:solidFill>
-              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Weeks</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="E8E8E8"/>
-            </a:solidFill>
-            <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>147825</xdr:colOff>
+      <xdr:colOff>1028887</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>566925</xdr:colOff>
+      <xdr:colOff>295462</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -1172,7 +832,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3195825" y="1857375"/>
+          <a:off x="3467287" y="1857375"/>
           <a:ext cx="1638300" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1263,429 +923,1071 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>353794</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>216712</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>6451</xdr:rowOff>
+      <xdr:colOff>360956</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>92176</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[0]!ShtMain.BtnLvl1Click" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="BtnLvl1">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="29" name="Group 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5296723A-A2C6-44B9-98ED-4EC22D98E06A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E46F923E-A190-4845-8898-D24C699E6D45}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4481512" y="742951"/>
-          <a:ext cx="612000" cy="216000"/>
+          <a:off x="2792194" y="742951"/>
+          <a:ext cx="2988487" cy="873225"/>
+          <a:chOff x="2647950" y="742951"/>
+          <a:chExt cx="2988487" cy="873225"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="DA2C38"/>
-              </a:solidFill>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="27" name="Group 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F72742C3-A38D-4288-894B-EE12AEC920C7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2647950" y="742951"/>
+            <a:ext cx="1323975" cy="647700"/>
+            <a:chOff x="2647950" y="771526"/>
+            <a:chExt cx="1323975" cy="647700"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="[0]!ShtMain.BtnLAR4wClick" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="BtnLAR4w">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711CF68E-298B-4110-AF75-6C65B51F5C08}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2647950" y="1095376"/>
+              <a:ext cx="1323975" cy="323850"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="DA2C38"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="DA2C38"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
               <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                  <a:prstClr val="black">
-                    <a:alpha val="50000"/>
-                  </a:prstClr>
-                </a:innerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                <a:prstClr val="black">
+                  <a:alpha val="50000"/>
+                </a:prstClr>
+              </a:innerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:srgbClr val="756A6D"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t> Weeks</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1000" b="0">
+                <a:solidFill>
+                  <a:srgbClr val="E8E8E8"/>
+                </a:solidFill>
+                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="[0]!ShtMain.BtnLAR12wClick" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="BtnLAR12w">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{764C1C12-42C1-4E22-9956-6BC2FBCAE756}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2647950" y="771526"/>
+              <a:ext cx="1323975" cy="323850"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:srgbClr val="DA2C38"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                      <a:prstClr val="black">
+                        <a:alpha val="50000"/>
+                      </a:prstClr>
+                    </a:innerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>12</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t> Weeks</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1000" b="0">
+                <a:solidFill>
+                  <a:srgbClr val="E8E8E8"/>
+                </a:solidFill>
+                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="28" name="Group 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6421550B-A380-4E30-A0CB-345C27089AC2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="5024437" y="742951"/>
+            <a:ext cx="612000" cy="873225"/>
+            <a:chOff x="5024437" y="742951"/>
+            <a:chExt cx="612000" cy="873225"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="[0]!ShtMain.BtnLvl1Click" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="BtnLvl1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5296723A-A2C6-44B9-98ED-4EC22D98E06A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5024437" y="742951"/>
+              <a:ext cx="612000" cy="216000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:srgbClr val="DA2C38"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                      <a:prstClr val="black">
+                        <a:alpha val="50000"/>
+                      </a:prstClr>
+                    </a:innerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>1</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="[0]!ShtMain.BtnLvl2Click" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="BtnLvl2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9DD6C83-F973-42BC-BFFF-2FD26F7C0FCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5024437" y="962026"/>
+              <a:ext cx="612000" cy="216000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="DA2C38"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="DA2C38"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                <a:prstClr val="black">
+                  <a:alpha val="50000"/>
+                </a:prstClr>
+              </a:innerShdw>
+            </a:effectLst>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:srgbClr val="756A6D"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>2</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="[0]!ShtMain.BtnLvl3Click" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="BtnLvl3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2545847-4DA1-41A9-8666-8A9E227321BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5024437" y="1181101"/>
+              <a:ext cx="612000" cy="216000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:srgbClr val="DA2C38"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                      <a:prstClr val="black">
+                        <a:alpha val="50000"/>
+                      </a:prstClr>
+                    </a:innerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>3</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="[0]!ShtMain.BtnLvl4Click" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="BtnLvl4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC192345-61AB-41EF-86A8-DA9449DF816E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5024437" y="1400176"/>
+              <a:ext cx="612000" cy="216000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="8A7E81"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:srgbClr val="DA2C38"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                      <a:prstClr val="black">
+                        <a:alpha val="50000"/>
+                      </a:prstClr>
+                    </a:innerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>4</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="18" name="Group 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98DC4614-1EDB-41D2-8B68-C2ADF3D8CEDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6419851" y="142875"/>
+          <a:ext cx="1504950" cy="2286000"/>
+          <a:chOff x="2466975" y="142875"/>
+          <a:chExt cx="3096000" cy="2286000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Rectangle: Rounded Corners 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B87121B0-8308-43F0-A59F-5B5E4D17DF17}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2466975" y="142875"/>
+            <a:ext cx="3096000" cy="2286000"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 2500"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="6D6A75"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-GB" sz="1100">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="Rectangle: Rounded Corners 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCBCAF10-6412-4606-B684-3C9451E32D04}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2466975" y="142875"/>
+            <a:ext cx="3096000" cy="352425"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="DA2C38"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100">
+                <a:solidFill>
+                  <a:srgbClr val="E8E8E8"/>
+                </a:solidFill>
+                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Export</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="E8E8E8"/>
+                </a:solidFill>
+                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> to PPT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100">
               <a:solidFill>
                 <a:srgbClr val="E8E8E8"/>
               </a:solidFill>
               <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>16764</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>216712</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>35026</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>440439</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[0]!ShtMain.BtnLvl2Click" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="BtnLvl2">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="Group 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9DD6C83-F973-42BC-BFFF-2FD26F7C0FCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693420D1-F772-42D5-A2C3-E96ABC15C05A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4481512" y="962026"/>
-          <a:ext cx="612000" cy="216000"/>
+          <a:off x="6655689" y="742950"/>
+          <a:ext cx="1033275" cy="1428749"/>
+          <a:chOff x="6655689" y="742950"/>
+          <a:chExt cx="1033275" cy="1428749"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="DA2C38"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="DA2C38"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-            <a:prstClr val="black">
-              <a:alpha val="50000"/>
-            </a:prstClr>
-          </a:innerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="756A6D"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
+      </xdr:grpSpPr>
+      <xdr:sp macro="[0]!ShtMain.BtnPPTExpClick" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="BtnPPTExp">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B718729A-B0CA-4A79-95F8-85327768039B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6655689" y="742950"/>
+            <a:ext cx="1033275" cy="1428749"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+            <a:tileRect/>
+          </a:gradFill>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="800000"/>
+          </a:ln>
+          <a:effectLst/>
+          <a:extLst>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="DA2C38"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a14:hiddenLine>
+            </a:ext>
+            <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+              <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:effectLst>
+                  <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                    <a:prstClr val="black">
+                      <a:alpha val="50000"/>
+                    </a:prstClr>
+                  </a:innerShdw>
+                </a:effectLst>
+              </a14:hiddenEffects>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:endParaRPr lang="en-GB" sz="1000" b="0">
               <a:solidFill>
                 <a:srgbClr val="E8E8E8"/>
               </a:solidFill>
               <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>2</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>216712</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>63601</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!ShtMain.BtnLvl3Click" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="BtnLvl3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2545847-4DA1-41A9-8666-8A9E227321BC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4481512" y="1181101"/>
-          <a:ext cx="612000" cy="216000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="DA2C38"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                  <a:prstClr val="black">
-                    <a:alpha val="50000"/>
-                  </a:prstClr>
-                </a:innerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="E8E8E8"/>
-              </a:solidFill>
-              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>3</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>216712</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92176</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!ShtMain.BtnLvl4Click" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="BtnLvl4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC192345-61AB-41EF-86A8-DA9449DF816E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4481512" y="1400176"/>
-          <a:ext cx="612000" cy="216000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="8A7E81"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="DA2C38"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                  <a:prstClr val="black">
-                    <a:alpha val="50000"/>
-                  </a:prstClr>
-                </a:innerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="E8E8E8"/>
-              </a:solidFill>
-              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>4</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="25" name="Group 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B58000D-7E8C-4EE1-9303-BA1C7FE7E540}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6822882" y="1114424"/>
+            <a:ext cx="698889" cy="685801"/>
+            <a:chOff x="6904952" y="1266824"/>
+            <a:chExt cx="699475" cy="685801"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="[0]!ShtMain.BtnPPTExpClick" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Rectangle 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393EBADE-24F4-4348-8E91-C736AF7DEF56}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7178386" y="1350818"/>
+              <a:ext cx="419966" cy="497898"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic macro="[0]!ShtMain.BtnPPTExpClick">
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Picture 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DF534D9-F7C9-483E-A14A-88E4F5270B61}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+              <a:clrChange>
+                <a:clrFrom>
+                  <a:srgbClr val="000000"/>
+                </a:clrFrom>
+                <a:clrTo>
+                  <a:srgbClr val="000000">
+                    <a:alpha val="0"/>
+                  </a:srgbClr>
+                </a:clrTo>
+              </a:clrChange>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6904952" y="1266824"/>
+              <a:ext cx="699475" cy="685801"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1989,37 +2291,63 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB7A1B8-C6E8-4CC3-A91F-BC6D2D0C2290}">
   <sheetPr codeName="ShtMain"/>
-  <dimension ref="E4:T6"/>
+  <dimension ref="E3:U6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="9"/>
     <col min="5" max="5" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="19" width="9.140625" style="9"/>
-    <col min="20" max="20" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="9"/>
+    <col min="6" max="18" width="9.140625" style="9"/>
+    <col min="19" max="21" width="9.5703125" style="10" hidden="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="S3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" s="10">
+        <v>3</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E4" s="9" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="T4" s="10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="5:20" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="S5" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="T5" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="S6" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="T6" s="10" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2424,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:M2326">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND($D3="", $E3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2106,8 +2434,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DD502A-100B-4C83-8462-52618C3EDF0B}">
-  <sheetPr codeName="ShtTaskView2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1025049-5377-4528-830A-385D397B7D4D}">
+  <sheetPr codeName="ShtTaskView3"/>
   <dimension ref="C2:P28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2134,37 +2462,37 @@
   <sheetData>
     <row r="2" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
@@ -2172,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
@@ -2180,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
@@ -2188,7 +2516,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
@@ -2196,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P6" s="5"/>
     </row>
@@ -2205,7 +2533,7 @@
         <v>2</v>
       </c>
       <c r="N7" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P7" s="5"/>
     </row>
@@ -2214,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P8" s="5"/>
     </row>
@@ -2223,13 +2551,13 @@
         <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P9" s="6"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2247,16 +2575,16 @@
         <v>1421.875</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="P10" s="6"/>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2274,16 +2602,16 @@
         <v>1421.875</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N11" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="P11" s="6"/>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2301,16 +2629,16 @@
         <v>1421.875</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N12" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="P12" s="6"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2328,16 +2656,16 @@
         <v>1421.875</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N13" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2355,16 +2683,16 @@
         <v>1421.875</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N14" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="P14" s="6"/>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2382,10 +2710,10 @@
         <v>1421.875</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N15" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="P15" s="6"/>
     </row>
@@ -2394,7 +2722,7 @@
         <v>24</v>
       </c>
       <c r="N16" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P16" s="6"/>
     </row>
@@ -2403,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
@@ -2411,7 +2739,7 @@
         <v>33</v>
       </c>
       <c r="N18" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
@@ -2419,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
@@ -2427,7 +2755,7 @@
         <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
@@ -2435,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.25">
@@ -2443,7 +2771,7 @@
         <v>37</v>
       </c>
       <c r="N22" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.25">
@@ -2451,15 +2779,15 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="N24" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.25">
@@ -2467,15 +2795,15 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="N26" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.25">
@@ -2483,20 +2811,20 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="N28" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:M2326">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($D3="", $E3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2506,8 +2834,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75031668-3A53-4F1E-8A3D-09DD02EC056B}">
-  <sheetPr codeName="ShtTaskView3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCF1581-DD8A-4532-B0AC-A15EE9D33AC2}">
+  <sheetPr codeName="ShtTaskView4"/>
   <dimension ref="C2:P46"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2534,37 +2862,37 @@
   <sheetData>
     <row r="2" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
@@ -2572,7 +2900,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
@@ -2580,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
@@ -2588,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
@@ -2596,7 +2924,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P6" s="5"/>
     </row>
@@ -2605,7 +2933,7 @@
         <v>2</v>
       </c>
       <c r="N7" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P7" s="5"/>
     </row>
@@ -2614,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P8" s="5"/>
     </row>
@@ -2623,13 +2951,13 @@
         <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P9" s="6"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2647,16 +2975,16 @@
         <v>1421.875</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N10" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P10" s="6"/>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2674,16 +3002,16 @@
         <v>1421.875</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P11" s="6"/>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2701,10 +3029,10 @@
         <v>1421.875</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N12" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P12" s="6"/>
     </row>
@@ -2728,10 +3056,10 @@
         <v>1421.875</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N13" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P13" s="6"/>
     </row>
@@ -2755,10 +3083,10 @@
         <v>1421.875</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N14" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P14" s="6"/>
     </row>
@@ -2782,10 +3110,10 @@
         <v>1421.875</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N15" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P15" s="6"/>
     </row>
@@ -2809,10 +3137,10 @@
         <v>1421.875</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N16" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P16" s="6"/>
     </row>
@@ -2836,10 +3164,10 @@
         <v>1421.875</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N17" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
@@ -2862,10 +3190,10 @@
         <v>1421.875</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N18" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
@@ -2888,10 +3216,10 @@
         <v>1421.875</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N19" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
@@ -2914,10 +3242,10 @@
         <v>1421.875</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N20" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
@@ -2940,10 +3268,10 @@
         <v>1421.875</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N21" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
@@ -2966,10 +3294,10 @@
         <v>1421.875</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N22" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
@@ -2992,10 +3320,10 @@
         <v>1421.875</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N23" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
@@ -3003,7 +3331,7 @@
         <v>24</v>
       </c>
       <c r="N24" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
@@ -3026,10 +3354,10 @@
         <v>1421.875</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N25" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
@@ -3052,10 +3380,10 @@
         <v>1421.875</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N26" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
@@ -3078,10 +3406,10 @@
         <v>1421.875</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N27" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.25">
@@ -3104,10 +3432,10 @@
         <v>1421.875</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N28" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
@@ -3130,10 +3458,10 @@
         <v>1421.875</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N29" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.25">
@@ -3156,10 +3484,10 @@
         <v>1421.875</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N30" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.25">
@@ -3182,10 +3510,10 @@
         <v>1417.5</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N31" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.25">
@@ -3208,10 +3536,10 @@
         <v>1417.5</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N32" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.25">
@@ -3219,7 +3547,7 @@
         <v>33</v>
       </c>
       <c r="N33" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
@@ -3242,10 +3570,10 @@
         <v>1417.5</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N34" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
@@ -3268,10 +3596,10 @@
         <v>1417.5</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N35" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
@@ -3279,7 +3607,7 @@
         <v>36</v>
       </c>
       <c r="N36" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
@@ -3287,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
@@ -3295,7 +3623,7 @@
         <v>37</v>
       </c>
       <c r="N38" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.25">
@@ -3318,10 +3646,10 @@
         <v>1417.5</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N39" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.25">
@@ -3344,10 +3672,10 @@
         <v>1417.5</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N40" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
@@ -3370,18 +3698,18 @@
         <v>1417.5</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N41" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="N42" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.25">
@@ -3389,15 +3717,15 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="N44" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.25">
@@ -3405,20 +3733,20 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="N46" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:M2326">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND($D3="", $E3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3428,8 +3756,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F1DED6-7031-431B-A91D-8255B09F3654}">
-  <sheetPr codeName="ShtTaskView4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26528467-A5BF-4C6A-98D0-7A0E18996B68}">
+  <sheetPr codeName="ShtTaskView5"/>
   <dimension ref="C2:P25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3456,37 +3784,37 @@
   <sheetData>
     <row r="2" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
@@ -3494,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
@@ -3502,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
@@ -3510,7 +3838,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
@@ -3518,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P6" s="5"/>
     </row>
@@ -3527,7 +3855,7 @@
         <v>2</v>
       </c>
       <c r="N7" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P7" s="5"/>
     </row>
@@ -3536,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P8" s="5"/>
     </row>
@@ -3545,7 +3873,7 @@
         <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P9" s="6"/>
     </row>
@@ -3554,7 +3882,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P10" s="6"/>
     </row>
@@ -3563,7 +3891,7 @@
         <v>24</v>
       </c>
       <c r="N11" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P11" s="6"/>
     </row>
@@ -3572,7 +3900,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P12" s="6"/>
     </row>
@@ -3581,7 +3909,7 @@
         <v>33</v>
       </c>
       <c r="N13" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P13" s="6"/>
     </row>
@@ -3590,7 +3918,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P14" s="6"/>
     </row>
@@ -3599,7 +3927,7 @@
         <v>36</v>
       </c>
       <c r="N15" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="P15" s="6"/>
     </row>
@@ -3608,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="P16" s="6"/>
     </row>
@@ -3617,12 +3945,12 @@
         <v>37</v>
       </c>
       <c r="N17" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3640,10 +3968,10 @@
         <v>1417.5</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N18" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
@@ -3666,18 +3994,18 @@
         <v>1417.5</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N19" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="N20" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
@@ -3700,10 +4028,10 @@
         <v>1417.5</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N21" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
@@ -3726,18 +4054,18 @@
         <v>1417.5</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="N22" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="N23" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
@@ -3745,1015 +4073,15 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="N25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C3:M2326">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>AND($D3="", $E3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4F915C-72B0-4110-A710-02AAA3A23FC7}">
-  <sheetPr codeName="ShtTaskView5"/>
-  <dimension ref="C2:P35"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>97</v>
-      </c>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
-        <v>95</v>
-      </c>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
-      </c>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" t="s">
-        <v>95</v>
-      </c>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>97</v>
-      </c>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" t="s">
-        <v>95</v>
-      </c>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>97</v>
-      </c>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" t="s">
-        <v>95</v>
-      </c>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>97</v>
-      </c>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" t="s">
-        <v>95</v>
-      </c>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>97</v>
-      </c>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>96</v>
-      </c>
-      <c r="N19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>-90007</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G20" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H20" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>-90008</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G21" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H21" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>-90009</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G22" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H22" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>-90010</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G23" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H23" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <v>-90011</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G24" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H24" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <v>-90012</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G25" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H25" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <v>-90013</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G26" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H26" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>-90014</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G27" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H27" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>-90015</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G28" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H28" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <v>-90016</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G29" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H29" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <v>-90017</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G30" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H30" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>-90018</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G31" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H31" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C32">
-        <v>-90019</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G32" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H32" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>63</v>
-      </c>
-      <c r="N33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
-        <v>66</v>
-      </c>
-      <c r="N35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C3:M2326">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND($D3="", $E3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F50629F-1633-4901-A845-653FC5ABBA9C}">
-  <sheetPr codeName="ShtTaskView6"/>
-  <dimension ref="C2:P28"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>97</v>
-      </c>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
-        <v>95</v>
-      </c>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
-      </c>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" t="s">
-        <v>95</v>
-      </c>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>97</v>
-      </c>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" t="s">
-        <v>95</v>
-      </c>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>97</v>
-      </c>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" t="s">
-        <v>95</v>
-      </c>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>97</v>
-      </c>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" t="s">
-        <v>95</v>
-      </c>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>97</v>
-      </c>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>96</v>
-      </c>
-      <c r="N19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>-90020</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G20" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H20" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G21" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H21" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G22" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H22" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>-90021</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G23" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H23" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <v>-90021.5</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G24" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H24" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>63</v>
-      </c>
-      <c r="N25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <v>-90022</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G26" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H26" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>-90023</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="4">
-        <v>43987</v>
-      </c>
-      <c r="G27" s="4">
-        <v>44022</v>
-      </c>
-      <c r="H27" s="8">
-        <v>1443.75</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
-        <v>66</v>
-      </c>
-      <c r="N28" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amended mapping from Tommi fixed raw data tab rename bug
</commit_message>
<xml_diff>
--- a/MSP Reporting Tool.xlsx
+++ b/MSP Reporting Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Development Areas\MSP Reporting Tool\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7A7C8BF-B790-490E-BC3B-F611042518AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E91A35F-9FD0-4897-B1C2-87CE86E872C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F7485911-4FC0-4026-A472-9F894C577CCD}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Dependancy Report" sheetId="248" r:id="rId2"/>
     <sheet name="Consolidated  Exception Report " sheetId="245" r:id="rId3"/>
-    <sheet name="Raw Plan Data" sheetId="227" r:id="rId4"/>
+    <sheet name="Plan Data" sheetId="227" r:id="rId4"/>
     <sheet name="Look Ahead Report" sheetId="246" state="hidden" r:id="rId5"/>
   </sheets>
   <externalReferences>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="54">
   <si>
     <t>DTI</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>Project</t>
-  </si>
-  <si>
-    <t>C:\Users\Julian\OneDrive\Documents\OneSheet\titilayo ilesanmi\Planning template v3.1.mpp</t>
   </si>
   <si>
     <t>Business Milestones</t>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>C:\Users\Julian\OneDrive\Documents\OneSheet\titilayo ilesanmi\Planning template v3.0.mpp</t>
   </si>
 </sst>
 </file>
@@ -921,7 +921,7 @@
         <xdr:cNvPr id="27" name="Group 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{485D412B-C307-4E6D-BFD6-85472D0E6746}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1760,10 +1760,10 @@
             <a:gradFill flip="none" rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:srgbClr val="DA2C38"/>
+                  <a:srgbClr val="8A7E81"/>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:srgbClr val="DA2C38"/>
+                  <a:srgbClr val="8A7E81"/>
                 </a:gs>
               </a:gsLst>
               <a:lin ang="5400000" scaled="1"/>
@@ -1774,22 +1774,27 @@
               <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst>
-              <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                <a:prstClr val="black">
-                  <a:alpha val="50000"/>
-                </a:prstClr>
-              </a:innerShdw>
-            </a:effectLst>
+            <a:effectLst/>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
                   <a:solidFill>
-                    <a:srgbClr val="756A6D"/>
+                    <a:srgbClr val="DA2C38"/>
                   </a:solidFill>
                   <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                 </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                      <a:prstClr val="black">
+                        <a:alpha val="50000"/>
+                      </a:prstClr>
+                    </a:innerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -2127,10 +2132,10 @@
             <a:gradFill flip="none" rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
+                  <a:srgbClr val="DA2C38"/>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
+                  <a:srgbClr val="DA2C38"/>
                 </a:gs>
               </a:gsLst>
               <a:lin ang="5400000" scaled="1"/>
@@ -2141,27 +2146,22 @@
               <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                <a:prstClr val="black">
+                  <a:alpha val="50000"/>
+                </a:prstClr>
+              </a:innerShdw>
+            </a:effectLst>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
                   <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
+                    <a:srgbClr val="756A6D"/>
                   </a:solidFill>
                   <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                 </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -2943,7 +2943,7 @@
         <xdr:cNvPr id="28" name="Group 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BB09AB6-D8D8-4EE9-951D-30CCC9F13FEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2962,7 +2962,7 @@
           <xdr:cNvPr id="38" name="Graphic 37" descr="Eraser">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74875FC2-F5DD-481C-87F2-32908EF0DA9F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3007,7 +3007,7 @@
           <xdr:cNvPr id="40" name="Rectangle: Rounded Corners 39">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C28AD200-52F7-4145-9542-CAA76F567ED1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -26119,7 +26119,7 @@
         <v>12</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="19:20">
@@ -26127,7 +26127,7 @@
         <v>3</v>
       </c>
       <c r="T5" s="4">
-        <v>1</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="6" spans="19:20">
@@ -26135,7 +26135,7 @@
         <v>13</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -26214,7 +26214,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="24.75" customHeight="1">
       <c r="A1" s="53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -26244,7 +26244,7 @@
     </row>
     <row r="2" spans="1:24" ht="29.25" customHeight="1">
       <c r="A2" s="56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57"/>
@@ -26253,7 +26253,7 @@
       <c r="F2" s="57"/>
       <c r="G2" s="58"/>
       <c r="H2" s="59" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="59"/>
       <c r="J2" s="59"/>
@@ -26262,11 +26262,11 @@
       <c r="M2" s="59"/>
       <c r="N2" s="59"/>
       <c r="O2" s="60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P2" s="60"/>
       <c r="Q2" s="61" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R2" s="61"/>
       <c r="S2" s="61"/>
@@ -26277,73 +26277,73 @@
     </row>
     <row r="3" spans="1:24" ht="25.5">
       <c r="A3" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="C3" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="D3" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="E3" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="F3" s="43" t="s">
         <v>41</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>42</v>
       </c>
       <c r="G3" s="44" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="46" t="s">
+      <c r="M3" s="46" t="s">
         <v>41</v>
-      </c>
-      <c r="M3" s="46" t="s">
-        <v>42</v>
       </c>
       <c r="N3" s="47" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P3" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" s="49" t="s">
+      <c r="R3" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="R3" s="50" t="s">
+      <c r="S3" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="S3" s="50" t="s">
+      <c r="T3" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="T3" s="50" t="s">
+      <c r="U3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="U3" s="50" t="s">
+      <c r="V3" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="V3" s="50" t="s">
+      <c r="W3" s="50" t="s">
         <v>50</v>
-      </c>
-      <c r="W3" s="50" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -26453,7 +26453,7 @@
     <col min="2" max="2" width="5.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.85546875" style="14" bestFit="1" customWidth="1"/>
@@ -26523,7 +26523,9 @@
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -26532,7 +26534,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="N3" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -26556,7 +26558,9 @@
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -26565,7 +26569,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="N5" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -26589,7 +26593,9 @@
       <c r="B7" s="16"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -26598,7 +26604,7 @@
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="N7" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -26622,7 +26628,9 @@
       <c r="B9" s="18"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="19"/>
+      <c r="E9" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -26631,7 +26639,7 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
       <c r="N9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -26656,559 +26664,694 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A9EE8F-EDC6-401D-AECC-57882115D77B}">
   <sheetPr codeName="ShtPlanData"/>
-  <dimension ref="F3:N136"/>
+  <dimension ref="E3:N136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="130.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:7">
+    <row r="3" spans="5:7">
+      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="6:7">
+    <row r="4" spans="5:7">
+      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="6:7">
+    <row r="5" spans="5:7">
+      <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="6:7">
+    <row r="6" spans="5:7">
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="6:7">
+    <row r="7" spans="5:7">
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="6:7">
+    <row r="8" spans="5:7">
+      <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="6:7">
+    <row r="9" spans="5:7">
+      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="6:7">
+    <row r="10" spans="5:7">
+      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="6:7">
+    <row r="11" spans="5:7">
+      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="6:7">
+    <row r="12" spans="5:7">
+      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="6:7">
+    <row r="13" spans="5:7">
+      <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="6:7">
+    <row r="14" spans="5:7">
+      <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="6:7">
+    <row r="15" spans="5:7">
+      <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="6:7">
+    <row r="16" spans="5:7">
+      <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="6:7">
+    <row r="17" spans="5:7">
+      <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="6:7">
+    <row r="18" spans="5:7">
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="6:7">
+    <row r="19" spans="5:7">
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="6:7">
+    <row r="20" spans="5:7">
+      <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="6:7">
+    <row r="21" spans="5:7">
+      <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="6:7">
+    <row r="22" spans="5:7">
+      <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="6:7">
+    <row r="23" spans="5:7">
+      <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="6:7">
+    <row r="24" spans="5:7">
+      <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="6:7">
+    <row r="25" spans="5:7">
+      <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="6:7">
+    <row r="26" spans="5:7">
+      <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="6:7">
+    <row r="27" spans="5:7">
+      <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="6:7">
+    <row r="28" spans="5:7">
+      <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="6:7">
+    <row r="29" spans="5:7">
+      <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="6:7">
+    <row r="30" spans="5:7">
+      <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="6:7">
+    <row r="31" spans="5:7">
+      <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="6:7">
+    <row r="32" spans="5:7">
+      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="6:7">
+    <row r="33" spans="5:7">
+      <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="6:7">
+    <row r="34" spans="5:7">
+      <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="6:7">
+    <row r="35" spans="5:7">
+      <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="6:7">
+    <row r="36" spans="5:7">
+      <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="6:7">
+    <row r="37" spans="5:7">
+      <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="6:7">
+    <row r="38" spans="5:7">
+      <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="6:7">
+    <row r="39" spans="5:7">
+      <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="6:7">
+    <row r="40" spans="5:7">
+      <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="6:7">
+    <row r="41" spans="5:7">
+      <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="6:7">
+    <row r="42" spans="5:7">
+      <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="6:7">
+    <row r="43" spans="5:7">
+      <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="6:7">
+    <row r="44" spans="5:7">
+      <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="6:7">
+    <row r="45" spans="5:7">
+      <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="6:7">
+    <row r="46" spans="5:7">
+      <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="6:7">
+    <row r="47" spans="5:7">
+      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="6:7">
+    <row r="48" spans="5:7">
+      <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="6:7">
+    <row r="49" spans="5:7">
+      <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="6:7">
+    <row r="50" spans="5:7">
+      <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="6:7">
+    <row r="51" spans="5:7">
+      <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="6:7">
+    <row r="52" spans="5:7">
+      <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="6:7">
+    <row r="53" spans="5:7">
+      <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="6:7">
+    <row r="54" spans="5:7">
+      <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="6:7">
+    <row r="55" spans="5:7">
+      <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="6:7">
+    <row r="56" spans="5:7">
+      <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="6:7">
+    <row r="57" spans="5:7">
+      <c r="E57" s="6"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="6:7">
+    <row r="58" spans="5:7">
+      <c r="E58" s="6"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="6:7">
+    <row r="59" spans="5:7">
+      <c r="E59" s="6"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="6:7">
+    <row r="60" spans="5:7">
+      <c r="E60" s="6"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="6:7">
+    <row r="61" spans="5:7">
+      <c r="E61" s="6"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="6:7">
+    <row r="62" spans="5:7">
+      <c r="E62" s="6"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="6:7">
+    <row r="63" spans="5:7">
+      <c r="E63" s="6"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="6:7">
+    <row r="64" spans="5:7">
+      <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="6:7">
+    <row r="65" spans="5:7">
+      <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="6:7">
+    <row r="66" spans="5:7">
+      <c r="E66" s="6"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="6:7">
+    <row r="67" spans="5:7">
+      <c r="E67" s="6"/>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="6:7">
+    <row r="68" spans="5:7">
+      <c r="E68" s="6"/>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="6:7">
+    <row r="69" spans="5:7">
+      <c r="E69" s="6"/>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="6:7">
+    <row r="70" spans="5:7">
+      <c r="E70" s="6"/>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="6:7">
+    <row r="71" spans="5:7">
+      <c r="E71" s="6"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="6:7">
+    <row r="72" spans="5:7">
+      <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="6:7">
+    <row r="73" spans="5:7">
+      <c r="E73" s="6"/>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="6:7">
+    <row r="74" spans="5:7">
+      <c r="E74" s="6"/>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="6:7">
+    <row r="75" spans="5:7">
+      <c r="E75" s="6"/>
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="6:7">
+    <row r="76" spans="5:7">
+      <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="6:7">
+    <row r="77" spans="5:7">
+      <c r="E77" s="6"/>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="6:7">
+    <row r="78" spans="5:7">
+      <c r="E78" s="6"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="6:7">
+    <row r="79" spans="5:7">
+      <c r="E79" s="6"/>
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="6:7">
+    <row r="80" spans="5:7">
+      <c r="E80" s="6"/>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="6:7">
+    <row r="81" spans="5:7">
+      <c r="E81" s="6"/>
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="6:7">
+    <row r="82" spans="5:7">
+      <c r="E82" s="6"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="6:7">
+    <row r="83" spans="5:7">
+      <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="6:7">
+    <row r="84" spans="5:7">
+      <c r="E84" s="6"/>
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="6:7">
+    <row r="85" spans="5:7">
+      <c r="E85" s="6"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="6:7">
+    <row r="86" spans="5:7">
+      <c r="E86" s="6"/>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="6:7">
+    <row r="87" spans="5:7">
+      <c r="E87" s="6"/>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="6:7">
+    <row r="88" spans="5:7">
+      <c r="E88" s="6"/>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="6:7">
+    <row r="89" spans="5:7">
+      <c r="E89" s="6"/>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="6:7">
+    <row r="90" spans="5:7">
+      <c r="E90" s="6"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="6:7">
+    <row r="91" spans="5:7">
+      <c r="E91" s="6"/>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="6:7">
+    <row r="92" spans="5:7">
+      <c r="E92" s="6"/>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="6:7">
+    <row r="93" spans="5:7">
+      <c r="E93" s="6"/>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="6:7">
+    <row r="94" spans="5:7">
+      <c r="E94" s="6"/>
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="6:7">
+    <row r="95" spans="5:7">
+      <c r="E95" s="6"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="6:7">
+    <row r="96" spans="5:7">
+      <c r="E96" s="6"/>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="6:7">
+    <row r="97" spans="5:7">
+      <c r="E97" s="6"/>
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="6:7">
+    <row r="98" spans="5:7">
+      <c r="E98" s="6"/>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="6:7">
+    <row r="99" spans="5:7">
+      <c r="E99" s="6"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
     </row>
-    <row r="100" spans="6:7">
+    <row r="100" spans="5:7">
+      <c r="E100" s="6"/>
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
     </row>
-    <row r="101" spans="6:7">
+    <row r="101" spans="5:7">
+      <c r="E101" s="6"/>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
     </row>
-    <row r="102" spans="6:7">
+    <row r="102" spans="5:7">
+      <c r="E102" s="6"/>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
     </row>
-    <row r="103" spans="6:7">
+    <row r="103" spans="5:7">
+      <c r="E103" s="6"/>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="6:7">
+    <row r="104" spans="5:7">
+      <c r="E104" s="6"/>
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
     </row>
-    <row r="105" spans="6:7">
+    <row r="105" spans="5:7">
+      <c r="E105" s="6"/>
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
     </row>
-    <row r="106" spans="6:7">
+    <row r="106" spans="5:7">
+      <c r="E106" s="6"/>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
     </row>
-    <row r="107" spans="6:7">
+    <row r="107" spans="5:7">
+      <c r="E107" s="6"/>
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
     </row>
-    <row r="108" spans="6:7">
+    <row r="108" spans="5:7">
+      <c r="E108" s="6"/>
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
     </row>
-    <row r="109" spans="6:7">
+    <row r="109" spans="5:7">
+      <c r="E109" s="6"/>
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
     </row>
-    <row r="110" spans="6:7">
+    <row r="110" spans="5:7">
+      <c r="E110" s="6"/>
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
     </row>
-    <row r="111" spans="6:7">
+    <row r="111" spans="5:7">
+      <c r="E111" s="6"/>
       <c r="F111" s="6"/>
       <c r="G111" s="6"/>
     </row>
-    <row r="112" spans="6:7">
+    <row r="112" spans="5:7">
+      <c r="E112" s="6"/>
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
     </row>
-    <row r="113" spans="6:7">
+    <row r="113" spans="5:7">
+      <c r="E113" s="6"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
     </row>
-    <row r="114" spans="6:7">
+    <row r="114" spans="5:7">
+      <c r="E114" s="6"/>
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
     </row>
-    <row r="115" spans="6:7">
+    <row r="115" spans="5:7">
+      <c r="E115" s="6"/>
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
     </row>
-    <row r="116" spans="6:7">
+    <row r="116" spans="5:7">
+      <c r="E116" s="6"/>
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
     </row>
-    <row r="117" spans="6:7">
+    <row r="117" spans="5:7">
+      <c r="E117" s="6"/>
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
     </row>
-    <row r="118" spans="6:7">
+    <row r="118" spans="5:7">
+      <c r="E118" s="6"/>
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
     </row>
-    <row r="119" spans="6:7">
+    <row r="119" spans="5:7">
+      <c r="E119" s="6"/>
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
     </row>
-    <row r="120" spans="6:7">
+    <row r="120" spans="5:7">
+      <c r="E120" s="6"/>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
     </row>
-    <row r="121" spans="6:7">
+    <row r="121" spans="5:7">
+      <c r="E121" s="6"/>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
     </row>
-    <row r="122" spans="6:7">
+    <row r="122" spans="5:7">
+      <c r="E122" s="6"/>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
     </row>
-    <row r="123" spans="6:7">
+    <row r="123" spans="5:7">
+      <c r="E123" s="6"/>
       <c r="F123" s="6"/>
       <c r="G123" s="6"/>
     </row>
-    <row r="124" spans="6:7">
+    <row r="124" spans="5:7">
+      <c r="E124" s="6"/>
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
     </row>
-    <row r="125" spans="6:7">
+    <row r="125" spans="5:7">
+      <c r="E125" s="6"/>
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
     </row>
-    <row r="126" spans="6:7">
+    <row r="126" spans="5:7">
+      <c r="E126" s="6"/>
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
     </row>
-    <row r="127" spans="6:7">
+    <row r="127" spans="5:7">
+      <c r="E127" s="6"/>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
     </row>
-    <row r="128" spans="6:7">
+    <row r="128" spans="5:7">
+      <c r="E128" s="6"/>
       <c r="F128" s="6"/>
       <c r="G128" s="6"/>
     </row>
-    <row r="129" spans="6:7">
+    <row r="129" spans="5:7">
+      <c r="E129" s="6"/>
       <c r="F129" s="6"/>
       <c r="G129" s="6"/>
     </row>
-    <row r="130" spans="6:7">
+    <row r="130" spans="5:7">
+      <c r="E130" s="6"/>
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
     </row>
-    <row r="131" spans="6:7">
+    <row r="131" spans="5:7">
+      <c r="E131" s="6"/>
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
     </row>
-    <row r="132" spans="6:7">
+    <row r="132" spans="5:7">
+      <c r="E132" s="6"/>
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
     </row>
-    <row r="133" spans="6:7">
+    <row r="133" spans="5:7">
+      <c r="E133" s="6"/>
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
     </row>
-    <row r="134" spans="6:7">
+    <row r="134" spans="5:7">
+      <c r="E134" s="6"/>
       <c r="F134" s="6"/>
       <c r="G134" s="6"/>
     </row>
-    <row r="135" spans="6:7">
+    <row r="135" spans="5:7">
+      <c r="E135" s="6"/>
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
     </row>
-    <row r="136" spans="6:7">
+    <row r="136" spans="5:7">
+      <c r="E136" s="6"/>
       <c r="F136" s="6"/>
       <c r="G136" s="6"/>
     </row>
@@ -27220,10 +27363,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688A652D-6DD1-48EF-B210-1032D24E28CA}">
   <sheetPr codeName="ShtTaskView"/>
-  <dimension ref="C2:P139"/>
+  <dimension ref="C2:P205"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15"/>
@@ -27241,7 +27384,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -27252,15 +27395,15 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="3:16">
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="3:16">
@@ -27268,15 +27411,15 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="3:16">
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="3:16">
@@ -27284,16 +27427,16 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P6" s="28"/>
     </row>
     <row r="7" spans="3:16">
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P7" s="28"/>
     </row>
@@ -27302,16 +27445,16 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P8" s="28"/>
     </row>
     <row r="9" spans="3:16">
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="29"/>
     </row>
@@ -27320,16 +27463,16 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P10" s="29"/>
     </row>
     <row r="11" spans="3:16">
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="29"/>
     </row>
@@ -27338,16 +27481,16 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P12" s="29"/>
     </row>
     <row r="13" spans="3:16">
       <c r="E13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P13" s="29"/>
     </row>
@@ -27356,16 +27499,16 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P14" s="29"/>
     </row>
     <row r="15" spans="3:16">
       <c r="E15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P15" s="29"/>
     </row>
@@ -27374,16 +27517,16 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P16" s="29"/>
     </row>
     <row r="17" spans="4:14">
       <c r="E17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="4:14">
@@ -27391,15 +27534,15 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="4:14">
       <c r="E19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:14">
@@ -27407,15 +27550,15 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="4:14">
       <c r="E21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="4:14">
@@ -27423,15 +27566,15 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="4:14">
       <c r="E23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="4:14">
@@ -27439,15 +27582,15 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="4:14">
       <c r="E25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="4:14">
@@ -27455,15 +27598,15 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="4:14">
       <c r="E27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="4:14">
@@ -27471,15 +27614,15 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="4:14">
       <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="N29" t="s">
         <v>30</v>
-      </c>
-      <c r="N29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="30" spans="4:14">
@@ -27487,15 +27630,15 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="4:14">
       <c r="E31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="4:14">
@@ -27503,15 +27646,15 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="4:14">
       <c r="E33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="4:14">
@@ -27519,15 +27662,15 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="4:14">
       <c r="E35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="4:14">
@@ -27535,15 +27678,15 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="4:14">
       <c r="E37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="4:14">
@@ -27551,15 +27694,15 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="4:14">
       <c r="E39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="4:14">
@@ -27567,15 +27710,15 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="4:14">
       <c r="E41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="4:14">
@@ -27583,15 +27726,15 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="4:14">
       <c r="E43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="4:14">
@@ -27599,15 +27742,15 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="4:14">
       <c r="E45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="4:14">
@@ -27615,15 +27758,15 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="4:14">
       <c r="E47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="4:14">
@@ -27631,15 +27774,15 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="4:14">
       <c r="E49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="4:14">
@@ -27647,15 +27790,15 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="4:14">
       <c r="E51" t="s">
+        <v>29</v>
+      </c>
+      <c r="N51" t="s">
         <v>30</v>
-      </c>
-      <c r="N51" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="52" spans="4:14">
@@ -27663,15 +27806,15 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="4:14">
       <c r="E53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="4:14">
@@ -27679,15 +27822,15 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="4:14">
       <c r="E55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="4:14">
@@ -27695,15 +27838,15 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="4:14">
       <c r="E57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="4:14">
@@ -27711,15 +27854,15 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="4:14">
       <c r="E59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="4:14">
@@ -27727,15 +27870,15 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="4:14">
       <c r="E61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="4:14">
@@ -27743,15 +27886,15 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="4:14">
       <c r="E63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="4:14">
@@ -27759,15 +27902,15 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="4:14">
       <c r="E65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="4:14">
@@ -27775,15 +27918,15 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="4:14">
       <c r="E67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="4:14">
@@ -27791,15 +27934,15 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="4:14">
       <c r="E69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="4:14">
@@ -27807,15 +27950,15 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="4:14">
       <c r="E71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="4:14">
@@ -27823,15 +27966,15 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="4:14">
       <c r="E73" t="s">
+        <v>29</v>
+      </c>
+      <c r="N73" t="s">
         <v>30</v>
-      </c>
-      <c r="N73" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="74" spans="4:14">
@@ -27839,15 +27982,15 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="4:14">
       <c r="E75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="4:14">
@@ -27855,15 +27998,15 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="4:14">
       <c r="E77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="4:14">
@@ -27871,15 +28014,15 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="4:14">
       <c r="E79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N79" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="4:14">
@@ -27887,15 +28030,15 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="81" spans="4:14">
       <c r="E81" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="4:14">
@@ -27903,15 +28046,15 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83" spans="4:14">
       <c r="E83" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="4:14">
@@ -27919,15 +28062,15 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="4:14">
       <c r="E85" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="4:14">
@@ -27935,15 +28078,15 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="4:14">
       <c r="E87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N87" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="4:14">
@@ -27951,15 +28094,15 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="4:14">
       <c r="E89" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="4:14">
@@ -27967,15 +28110,15 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="4:14">
       <c r="E91" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N91" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="4:14">
@@ -27983,15 +28126,15 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="4:14">
       <c r="E93" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N93" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="4:14">
@@ -27999,15 +28142,15 @@
         <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="4:14">
       <c r="E95" t="s">
+        <v>29</v>
+      </c>
+      <c r="N95" t="s">
         <v>30</v>
-      </c>
-      <c r="N95" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="96" spans="4:14">
@@ -28015,15 +28158,15 @@
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="4:14">
       <c r="E97" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="4:14">
@@ -28031,15 +28174,15 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="99" spans="4:14">
       <c r="E99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N99" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="100" spans="4:14">
@@ -28047,15 +28190,15 @@
         <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="101" spans="4:14">
       <c r="E101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N101" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="4:14">
@@ -28063,15 +28206,15 @@
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="103" spans="4:14">
       <c r="E103" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N103" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="104" spans="4:14">
@@ -28079,15 +28222,15 @@
         <v>0</v>
       </c>
       <c r="E104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="105" spans="4:14">
       <c r="E105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N105" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="106" spans="4:14">
@@ -28095,15 +28238,15 @@
         <v>0</v>
       </c>
       <c r="E106" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="107" spans="4:14">
       <c r="E107" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N107" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="4:14">
@@ -28111,15 +28254,15 @@
         <v>0</v>
       </c>
       <c r="E108" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109" spans="4:14">
       <c r="E109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N109" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110" spans="4:14">
@@ -28127,15 +28270,15 @@
         <v>0</v>
       </c>
       <c r="E110" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="111" spans="4:14">
       <c r="E111" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N111" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="4:14">
@@ -28143,15 +28286,15 @@
         <v>0</v>
       </c>
       <c r="E112" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="113" spans="4:14">
       <c r="E113" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N113" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="114" spans="4:14">
@@ -28159,15 +28302,15 @@
         <v>0</v>
       </c>
       <c r="E114" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="115" spans="4:14">
       <c r="E115" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N115" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="116" spans="4:14">
@@ -28175,15 +28318,15 @@
         <v>0</v>
       </c>
       <c r="E116" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="117" spans="4:14">
       <c r="E117" t="s">
+        <v>29</v>
+      </c>
+      <c r="N117" t="s">
         <v>30</v>
-      </c>
-      <c r="N117" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="118" spans="4:14">
@@ -28191,15 +28334,15 @@
         <v>0</v>
       </c>
       <c r="E118" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="4:14">
       <c r="E119" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N119" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="120" spans="4:14">
@@ -28207,15 +28350,15 @@
         <v>0</v>
       </c>
       <c r="E120" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="121" spans="4:14">
       <c r="E121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N121" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122" spans="4:14">
@@ -28223,15 +28366,15 @@
         <v>0</v>
       </c>
       <c r="E122" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" spans="4:14">
       <c r="E123" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N123" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="124" spans="4:14">
@@ -28239,15 +28382,15 @@
         <v>0</v>
       </c>
       <c r="E124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="125" spans="4:14">
       <c r="E125" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N125" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126" spans="4:14">
@@ -28255,15 +28398,15 @@
         <v>0</v>
       </c>
       <c r="E126" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="127" spans="4:14">
       <c r="E127" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N127" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="128" spans="4:14">
@@ -28271,15 +28414,15 @@
         <v>0</v>
       </c>
       <c r="E128" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129" spans="4:14">
       <c r="E129" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N129" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="130" spans="4:14">
@@ -28287,15 +28430,15 @@
         <v>0</v>
       </c>
       <c r="E130" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="131" spans="4:14">
       <c r="E131" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N131" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="132" spans="4:14">
@@ -28303,15 +28446,15 @@
         <v>0</v>
       </c>
       <c r="E132" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="133" spans="4:14">
       <c r="E133" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N133" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="4:14">
@@ -28319,15 +28462,15 @@
         <v>0</v>
       </c>
       <c r="E134" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="4:14">
       <c r="E135" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N135" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="4:14">
@@ -28335,15 +28478,15 @@
         <v>0</v>
       </c>
       <c r="E136" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="137" spans="4:14">
       <c r="E137" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N137" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="138" spans="4:14">
@@ -28351,15 +28494,543 @@
         <v>0</v>
       </c>
       <c r="E138" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="139" spans="4:14">
       <c r="E139" t="s">
+        <v>29</v>
+      </c>
+      <c r="N139" t="s">
         <v>30</v>
       </c>
-      <c r="N139" t="s">
+    </row>
+    <row r="140" spans="4:14">
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="141" spans="4:14">
+      <c r="E141" t="s">
+        <v>19</v>
+      </c>
+      <c r="N141" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="142" spans="4:14">
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="143" spans="4:14">
+      <c r="E143" t="s">
+        <v>20</v>
+      </c>
+      <c r="N143" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="144" spans="4:14">
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="145" spans="4:14">
+      <c r="E145" t="s">
+        <v>21</v>
+      </c>
+      <c r="N145" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="146" spans="4:14">
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="147" spans="4:14">
+      <c r="E147" t="s">
+        <v>22</v>
+      </c>
+      <c r="N147" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="148" spans="4:14">
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="149" spans="4:14">
+      <c r="E149" t="s">
+        <v>23</v>
+      </c>
+      <c r="N149" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="150" spans="4:14">
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="151" spans="4:14">
+      <c r="E151" t="s">
+        <v>24</v>
+      </c>
+      <c r="N151" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="152" spans="4:14">
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="153" spans="4:14">
+      <c r="E153" t="s">
+        <v>25</v>
+      </c>
+      <c r="N153" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="154" spans="4:14">
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="155" spans="4:14">
+      <c r="E155" t="s">
+        <v>26</v>
+      </c>
+      <c r="N155" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="156" spans="4:14">
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="157" spans="4:14">
+      <c r="E157" t="s">
+        <v>27</v>
+      </c>
+      <c r="N157" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="158" spans="4:14">
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="159" spans="4:14">
+      <c r="E159" t="s">
+        <v>28</v>
+      </c>
+      <c r="N159" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="160" spans="4:14">
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="161" spans="4:14">
+      <c r="E161" t="s">
+        <v>29</v>
+      </c>
+      <c r="N161" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="162" spans="4:14">
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="163" spans="4:14">
+      <c r="E163" t="s">
+        <v>19</v>
+      </c>
+      <c r="N163" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="164" spans="4:14">
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="165" spans="4:14">
+      <c r="E165" t="s">
+        <v>20</v>
+      </c>
+      <c r="N165" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="166" spans="4:14">
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="167" spans="4:14">
+      <c r="E167" t="s">
+        <v>21</v>
+      </c>
+      <c r="N167" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="168" spans="4:14">
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="169" spans="4:14">
+      <c r="E169" t="s">
+        <v>22</v>
+      </c>
+      <c r="N169" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="4:14">
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="171" spans="4:14">
+      <c r="E171" t="s">
+        <v>23</v>
+      </c>
+      <c r="N171" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="172" spans="4:14">
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="173" spans="4:14">
+      <c r="E173" t="s">
+        <v>24</v>
+      </c>
+      <c r="N173" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="174" spans="4:14">
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="175" spans="4:14">
+      <c r="E175" t="s">
+        <v>25</v>
+      </c>
+      <c r="N175" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="176" spans="4:14">
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="177" spans="4:14">
+      <c r="E177" t="s">
+        <v>26</v>
+      </c>
+      <c r="N177" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="178" spans="4:14">
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="179" spans="4:14">
+      <c r="E179" t="s">
+        <v>27</v>
+      </c>
+      <c r="N179" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="180" spans="4:14">
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="181" spans="4:14">
+      <c r="E181" t="s">
+        <v>28</v>
+      </c>
+      <c r="N181" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="182" spans="4:14">
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="183" spans="4:14">
+      <c r="E183" t="s">
+        <v>29</v>
+      </c>
+      <c r="N183" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="184" spans="4:14">
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="185" spans="4:14">
+      <c r="E185" t="s">
+        <v>19</v>
+      </c>
+      <c r="N185" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="186" spans="4:14">
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="187" spans="4:14">
+      <c r="E187" t="s">
+        <v>20</v>
+      </c>
+      <c r="N187" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="188" spans="4:14">
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="189" spans="4:14">
+      <c r="E189" t="s">
+        <v>21</v>
+      </c>
+      <c r="N189" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="190" spans="4:14">
+      <c r="D190">
+        <v>0</v>
+      </c>
+      <c r="E190" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="191" spans="4:14">
+      <c r="E191" t="s">
+        <v>22</v>
+      </c>
+      <c r="N191" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="192" spans="4:14">
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="193" spans="4:14">
+      <c r="E193" t="s">
+        <v>23</v>
+      </c>
+      <c r="N193" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="194" spans="4:14">
+      <c r="D194">
+        <v>0</v>
+      </c>
+      <c r="E194" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="195" spans="4:14">
+      <c r="E195" t="s">
+        <v>24</v>
+      </c>
+      <c r="N195" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="196" spans="4:14">
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="197" spans="4:14">
+      <c r="E197" t="s">
+        <v>25</v>
+      </c>
+      <c r="N197" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="198" spans="4:14">
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="199" spans="4:14">
+      <c r="E199" t="s">
+        <v>26</v>
+      </c>
+      <c r="N199" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="200" spans="4:14">
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="201" spans="4:14">
+      <c r="E201" t="s">
+        <v>27</v>
+      </c>
+      <c r="N201" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="202" spans="4:14">
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="203" spans="4:14">
+      <c r="E203" t="s">
+        <v>28</v>
+      </c>
+      <c r="N203" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="204" spans="4:14">
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="205" spans="4:14">
+      <c r="E205" t="s">
+        <v>29</v>
+      </c>
+      <c r="N205" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started moving LAH and levels to apply to all reports
</commit_message>
<xml_diff>
--- a/MSP Reporting Tool.xlsx
+++ b/MSP Reporting Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Development Areas\MSP Reporting Tool\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E91A35F-9FD0-4897-B1C2-87CE86E872C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{071CE4CA-134E-4ABF-A17F-77153260AD66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F7485911-4FC0-4026-A472-9F894C577CCD}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="54">
   <si>
     <t>DTI</t>
   </si>
@@ -905,23 +905,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>116651</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>167663</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293489</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>161440</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>384652</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>100988</xdr:rowOff>
+      <xdr:rowOff>145744</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="27" name="Group 26">
+        <xdr:cNvPr id="59" name="Group 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{379D7F37-F27E-4213-8CDD-A8F9CB16C2C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -929,10 +929,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="726251" y="739163"/>
-          <a:ext cx="654389" cy="885825"/>
-          <a:chOff x="792645" y="739163"/>
-          <a:chExt cx="654389" cy="885825"/>
+          <a:off x="1512689" y="764869"/>
+          <a:ext cx="700763" cy="904875"/>
+          <a:chOff x="726250" y="739163"/>
+          <a:chExt cx="700763" cy="904875"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic macro="[0]!ShtMain.BtnImportClick">
@@ -963,8 +963,8 @@
         </xdr:blipFill>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="792645" y="739163"/>
-            <a:ext cx="654389" cy="571500"/>
+            <a:off x="726250" y="739163"/>
+            <a:ext cx="700763" cy="612000"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -1001,7 +1001,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="795839" y="1367813"/>
+            <a:off x="752631" y="1386863"/>
             <a:ext cx="648000" cy="257175"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -1065,23 +1065,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>93844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>352426</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>49575</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>320400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>16669</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="24" name="Group 23">
+        <xdr:cNvPr id="1032" name="Group 1031">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178D2749-A8DC-4720-8DF4-F7E66ACD7230}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1089,18 +1089,18 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9144001" y="219075"/>
-          <a:ext cx="1504950" cy="1926000"/>
-          <a:chOff x="8582026" y="161925"/>
-          <a:chExt cx="1504950" cy="1926000"/>
+          <a:off x="2676525" y="474844"/>
+          <a:ext cx="4892400" cy="1446825"/>
+          <a:chOff x="1866900" y="751069"/>
+          <a:chExt cx="4892400" cy="1446825"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="19" name="Rectangle: Rounded Corners 18">
+          <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1108,8 +1108,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8582026" y="161925"/>
-            <a:ext cx="1504950" cy="1926000"/>
+            <a:off x="1866900" y="751069"/>
+            <a:ext cx="4892400" cy="1446825"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst>
@@ -1159,12 +1159,962 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="Rectangle: Rounded Corners 19">
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="1031" name="Group 1030">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A9B811-937F-4523-9472-AA157B706B73}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1866900" y="751069"/>
+            <a:ext cx="4892400" cy="1300619"/>
+            <a:chOff x="1866900" y="751069"/>
+            <a:chExt cx="4892400" cy="1300619"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1866900" y="751069"/>
+              <a:ext cx="4892400" cy="352425"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="DA2C38"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Report Settings</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="1030" name="Group 1029">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691ABE72-36A3-44B0-B3A5-49CE86D5C536}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="2503540" y="1163025"/>
+              <a:ext cx="3638171" cy="888663"/>
+              <a:chOff x="2379714" y="1163025"/>
+              <a:chExt cx="3876296" cy="888663"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="1027" name="Group 1026">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D730A2-18AE-4E74-9D29-78955242BB77}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="4788860" y="1163025"/>
+                <a:ext cx="1229025" cy="888663"/>
+                <a:chOff x="5226823" y="1163025"/>
+                <a:chExt cx="1229025" cy="888663"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="3" name="Group 2">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34E8503A-BAF8-44E8-8003-B2389828036D}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="5226823" y="1382101"/>
+                  <a:ext cx="1229025" cy="669587"/>
+                  <a:chOff x="3640415" y="772501"/>
+                  <a:chExt cx="1229025" cy="669587"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:sp macro="[0]!ShtMain.BtnLvl1Click" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="13" name="BtnLvl1">
+                    <a:extLst>
+                      <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:cNvPr>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="3640415" y="772501"/>
+                    <a:ext cx="612000" cy="216000"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:gradFill flip="none" rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="1"/>
+                    <a:tileRect/>
+                  </a:gradFill>
+                  <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+                    <a:noFill/>
+                    <a:prstDash val="solid"/>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst/>
+                  <a:extLst>
+                    <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                      <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                        <a:solidFill>
+                          <a:srgbClr val="DA2C38"/>
+                        </a:solidFill>
+                        <a:prstDash val="solid"/>
+                        <a:miter lim="800000"/>
+                      </a14:hiddenLine>
+                    </a:ext>
+                    <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                      <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                        <a:effectLst>
+                          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                            <a:prstClr val="black">
+                              <a:alpha val="50000"/>
+                            </a:prstClr>
+                          </a:innerShdw>
+                        </a:effectLst>
+                      </a14:hiddenEffects>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="1000" b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="E8E8E8"/>
+                        </a:solidFill>
+                        <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>1</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="[0]!ShtMain.BtnLvl2Click" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="14" name="BtnLvl2">
+                    <a:extLst>
+                      <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:cNvPr>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="3640415" y="1001101"/>
+                    <a:ext cx="612000" cy="216000"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:gradFill flip="none" rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="1"/>
+                    <a:tileRect/>
+                  </a:gradFill>
+                  <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+                    <a:noFill/>
+                    <a:prstDash val="solid"/>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst/>
+                  <a:extLst>
+                    <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                      <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                        <a:solidFill>
+                          <a:srgbClr val="DA2C38"/>
+                        </a:solidFill>
+                        <a:prstDash val="solid"/>
+                        <a:miter lim="800000"/>
+                      </a14:hiddenLine>
+                    </a:ext>
+                    <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                      <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                        <a:effectLst>
+                          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                            <a:prstClr val="black">
+                              <a:alpha val="50000"/>
+                            </a:prstClr>
+                          </a:innerShdw>
+                        </a:effectLst>
+                      </a14:hiddenEffects>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="1000" b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="E8E8E8"/>
+                        </a:solidFill>
+                        <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>2</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="[0]!ShtMain.BtnLvl3Click" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="15" name="BtnLvl3">
+                    <a:extLst>
+                      <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:cNvPr>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="4257440" y="772501"/>
+                    <a:ext cx="612000" cy="216000"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:gradFill flip="none" rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="1"/>
+                    <a:tileRect/>
+                  </a:gradFill>
+                  <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+                    <a:noFill/>
+                    <a:prstDash val="solid"/>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst/>
+                  <a:extLst>
+                    <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                      <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                        <a:solidFill>
+                          <a:srgbClr val="DA2C38"/>
+                        </a:solidFill>
+                        <a:prstDash val="solid"/>
+                        <a:miter lim="800000"/>
+                      </a14:hiddenLine>
+                    </a:ext>
+                    <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                      <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                        <a:effectLst>
+                          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                            <a:prstClr val="black">
+                              <a:alpha val="50000"/>
+                            </a:prstClr>
+                          </a:innerShdw>
+                        </a:effectLst>
+                      </a14:hiddenEffects>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="1000" b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="E8E8E8"/>
+                        </a:solidFill>
+                        <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>3</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="[0]!ShtMain.BtnLvl4Click" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="16" name="BtnLvl4">
+                    <a:extLst>
+                      <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:cNvPr>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="4257440" y="1001101"/>
+                    <a:ext cx="612000" cy="216000"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:gradFill flip="none" rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:srgbClr val="8A7E81"/>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="1"/>
+                    <a:tileRect/>
+                  </a:gradFill>
+                  <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+                    <a:noFill/>
+                    <a:prstDash val="solid"/>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst/>
+                  <a:extLst>
+                    <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                      <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                        <a:solidFill>
+                          <a:srgbClr val="DA2C38"/>
+                        </a:solidFill>
+                        <a:prstDash val="solid"/>
+                        <a:miter lim="800000"/>
+                      </a14:hiddenLine>
+                    </a:ext>
+                    <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                      <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                        <a:effectLst>
+                          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                            <a:prstClr val="black">
+                              <a:alpha val="50000"/>
+                            </a:prstClr>
+                          </a:innerShdw>
+                        </a:effectLst>
+                      </a14:hiddenEffects>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="1000" b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="E8E8E8"/>
+                        </a:solidFill>
+                        <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>4</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="[0]!ShtMain.BtnLvlAllClick" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="26" name="BtnLvlAll">
+                    <a:extLst>
+                      <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:cNvPr>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="3640415" y="1226088"/>
+                    <a:ext cx="1224000" cy="216000"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:gradFill flip="none" rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:srgbClr val="DA2C38"/>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:srgbClr val="DA2C38"/>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="1"/>
+                    <a:tileRect/>
+                  </a:gradFill>
+                  <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+                    <a:noFill/>
+                    <a:prstDash val="solid"/>
+                    <a:miter lim="800000"/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                      <a:prstClr val="black">
+                        <a:alpha val="50000"/>
+                      </a:prstClr>
+                    </a:innerShdw>
+                  </a:effectLst>
+                  <a:extLst>
+                    <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                      <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                        <a:solidFill>
+                          <a:srgbClr val="756A6D"/>
+                        </a:solidFill>
+                        <a:prstDash val="solid"/>
+                        <a:miter lim="800000"/>
+                      </a14:hiddenLine>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="1000" b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="E8E8E8"/>
+                        </a:solidFill>
+                        <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>All</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+            </xdr:grpSp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="23" name="TextBox 22">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="5507960" y="1163025"/>
+                  <a:ext cx="666750" cy="209550"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln w="9525" cmpd="sng">
+                  <a:noFill/>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100">
+                      <a:solidFill>
+                        <a:srgbClr val="E8E8E8"/>
+                      </a:solidFill>
+                    </a:rPr>
+                    <a:t>Level</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="1028" name="Group 1027">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A73762-BE00-44C5-8F62-AB2530848D4A}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="2379714" y="1335185"/>
+                <a:ext cx="1454424" cy="544343"/>
+                <a:chOff x="2084252" y="1334476"/>
+                <a:chExt cx="1454424" cy="544343"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="30" name="TextBox 29">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="2084252" y="1334476"/>
+                  <a:ext cx="1454424" cy="276224"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln w="9525" cmpd="sng">
+                  <a:noFill/>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr"/>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100">
+                      <a:solidFill>
+                        <a:srgbClr val="E8E8E8"/>
+                      </a:solidFill>
+                    </a:rPr>
+                    <a:t>Look Ahead</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="E8E8E8"/>
+                      </a:solidFill>
+                    </a:rPr>
+                    <a:t> (wks)</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100"/>
+                    <a:t> </a:t>
+                  </a:r>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+              <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+                <xdr:sp macro="" textlink="">
+                  <xdr:nvSpPr>
+                    <xdr:cNvPr id="1025" name="TxtLAValue" hidden="1">
+                      <a:extLst>
+                        <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                          <a14:compatExt spid="_x0000_s1025"/>
+                        </a:ext>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvSpPr/>
+                  </xdr:nvSpPr>
+                  <xdr:spPr bwMode="auto">
+                    <a:xfrm>
+                      <a:off x="2506664" y="1612119"/>
+                      <a:ext cx="609600" cy="266700"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:extLst>
+                      <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                        <a14:hiddenLine w="9525">
+                          <a:noFill/>
+                          <a:miter lim="800000"/>
+                          <a:headEnd/>
+                          <a:tailEnd/>
+                        </a14:hiddenLine>
+                      </a:ext>
+                    </a:extLst>
+                  </xdr:spPr>
+                </xdr:sp>
+              </mc:Choice>
+              <mc:Fallback/>
+            </mc:AlternateContent>
+          </xdr:grpSp>
+        </xdr:grpSp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>357970</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>184887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>74770</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>154226</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="63" name="Group 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB274197-BECF-4238-8D0C-B79BA161E0C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8216095" y="756387"/>
+          <a:ext cx="936000" cy="921839"/>
+          <a:chOff x="6158695" y="665049"/>
+          <a:chExt cx="936000" cy="921839"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="25" name="Group 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr>
+            <a:grpSpLocks noChangeAspect="1"/>
+          </xdr:cNvGrpSpPr>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6311565" y="665049"/>
+            <a:ext cx="630261" cy="612000"/>
+            <a:chOff x="6904952" y="1266824"/>
+            <a:chExt cx="699475" cy="685801"/>
+          </a:xfrm>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:grpSpPr>
+        <xdr:sp macro="[0]!ShtMain.BtnPPTExpClick" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Rectangle 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7178386" y="1350818"/>
+              <a:ext cx="419966" cy="497898"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic macro="[0]!ShtMain.BtnPPTExpClick">
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Picture 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+              <a:clrChange>
+                <a:clrFrom>
+                  <a:srgbClr val="000000"/>
+                </a:clrFrom>
+                <a:clrTo>
+                  <a:srgbClr val="000000">
+                    <a:alpha val="0"/>
+                  </a:srgbClr>
+                </a:clrTo>
+              </a:clrChange>
+              <a:duotone>
+                <a:prstClr val="black"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:tint val="45000"/>
+                  <a:satMod val="400000"/>
+                </a:schemeClr>
+              </a:duotone>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6904952" y="1266824"/>
+              <a:ext cx="699475" cy="685801"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+      <xdr:sp macro="[0]!ThisWorkbook.ClearData" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="Rectangle: Rounded Corners 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1172,18 +2122,25 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8582026" y="161925"/>
-            <a:ext cx="1504950" cy="352425"/>
+            <a:off x="6158695" y="1329713"/>
+            <a:ext cx="936000" cy="257175"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:srgbClr val="DA2C38"/>
+            <a:srgbClr val="6D6A75"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="2">
@@ -1205,24 +2162,15 @@
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="l"/>
+            <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="en-GB" sz="1100">
+              <a:rPr lang="en-GB" sz="1200">
                 <a:solidFill>
                   <a:srgbClr val="E8E8E8"/>
                 </a:solidFill>
                 <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Export</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="E8E8E8"/>
-                </a:solidFill>
-                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> to PPT</a:t>
+              <a:t>PPT Export</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1100">
               <a:solidFill>
@@ -1233,12 +2181,47 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>321950</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116025</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="1024" name="Group 1023">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB460F3A-4715-4C62-815E-D5F040790516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2676525" y="2105025"/>
+          <a:ext cx="4893950" cy="1440000"/>
+          <a:chOff x="2108825" y="2381250"/>
+          <a:chExt cx="4893950" cy="1440000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="Group 6">
+          <xdr:cNvPr id="55" name="Group 54">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33C47F0-EAFC-48CD-8816-E37AECDA53F4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1246,18 +2229,18 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="8817864" y="762001"/>
-            <a:ext cx="1033275" cy="1066800"/>
-            <a:chOff x="6655689" y="742951"/>
-            <a:chExt cx="1033275" cy="1066800"/>
+            <a:off x="2108825" y="2381250"/>
+            <a:ext cx="1504950" cy="1440000"/>
+            <a:chOff x="2032625" y="2381250"/>
+            <a:chExt cx="1504950" cy="1440000"/>
           </a:xfrm>
         </xdr:grpSpPr>
-        <xdr:sp macro="[0]!ShtMain.BtnPPTExpClick" textlink="">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="21" name="BtnPPTExp">
+            <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1265,8 +2248,131 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6655689" y="742951"/>
-              <a:ext cx="1033275" cy="1066800"/>
+              <a:off x="2032625" y="2381250"/>
+              <a:ext cx="1504950" cy="1440000"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst>
+                <a:gd name="adj" fmla="val 2500"/>
+              </a:avLst>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="6D6A75"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2032625" y="2381250"/>
+              <a:ext cx="1504950" cy="352425"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="DA2C38"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Exception Report</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="[0]!ShtMain.BtnExcRepGenClick" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="37" name="BtnExcRepGen">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2268500" y="3074650"/>
+              <a:ext cx="1033200" cy="323850"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1338,393 +2444,27 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr marL="0" indent="0" algn="ctr"/>
-              <a:endParaRPr lang="en-GB" sz="1000" b="0">
-                <a:solidFill>
-                  <a:srgbClr val="E8E8E8"/>
-                </a:solidFill>
-                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:endParaRPr>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>Generate</a:t>
+              </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="25" name="Group 24">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="6822882" y="933451"/>
-              <a:ext cx="698889" cy="685801"/>
-              <a:chOff x="6904952" y="1266824"/>
-              <a:chExt cx="699475" cy="685801"/>
-            </a:xfrm>
-          </xdr:grpSpPr>
-          <xdr:sp macro="[0]!ShtMain.BtnPPTExpClick" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="12" name="Rectangle 11">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="7178386" y="1350818"/>
-                <a:ext cx="419966" cy="497898"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-GB" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:pic macro="[0]!ShtMain.BtnPPTExpClick">
-            <xdr:nvPicPr>
-              <xdr:cNvPr id="11" name="Picture 10">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvPicPr>
-                <a:picLocks noChangeAspect="1"/>
-              </xdr:cNvPicPr>
-            </xdr:nvPicPr>
-            <xdr:blipFill>
-              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-                <a:clrChange>
-                  <a:clrFrom>
-                    <a:srgbClr val="000000"/>
-                  </a:clrFrom>
-                  <a:clrTo>
-                    <a:srgbClr val="000000">
-                      <a:alpha val="0"/>
-                    </a:srgbClr>
-                  </a:clrTo>
-                </a:clrChange>
-              </a:blip>
-              <a:stretch>
-                <a:fillRect/>
-              </a:stretch>
-            </xdr:blipFill>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="6904952" y="1266824"/>
-                <a:ext cx="699475" cy="685801"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-            </xdr:spPr>
-          </xdr:pic>
-        </xdr:grpSp>
       </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>29550</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>243825</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="9" name="Group 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1876425" y="220050"/>
-          <a:ext cx="3177525" cy="1924050"/>
-          <a:chOff x="2914650" y="142875"/>
-          <a:chExt cx="3177525" cy="1924050"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 4">
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="56" name="Group 55">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2924175" y="142875"/>
-            <a:ext cx="3168000" cy="1924050"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 2500"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="6D6A75"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-GB" sz="1100">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2914650" y="142875"/>
-            <a:ext cx="3168000" cy="352425"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="DA2C38"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="E8E8E8"/>
-                </a:solidFill>
-                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Look Ahead Report</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="[0]!ShtMain.BtnLARGenClick" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="BtnLARGen">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3140031" y="1498263"/>
-            <a:ext cx="1638300" cy="323850"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:gradFill flip="none" rotWithShape="1">
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:srgbClr val="8A7E81"/>
-              </a:gs>
-              <a:gs pos="100000">
-                <a:srgbClr val="8A7E81"/>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="5400000" scaled="1"/>
-            <a:tileRect/>
-          </a:gradFill>
-          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-            <a:noFill/>
-            <a:prstDash val="solid"/>
-            <a:miter lim="800000"/>
-          </a:ln>
-          <a:effectLst/>
-          <a:extLst>
-            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:srgbClr val="DA2C38"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:miter lim="800000"/>
-              </a14:hiddenLine>
-            </a:ext>
-            <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-              <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:effectLst>
-                  <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                    <a:prstClr val="black">
-                      <a:alpha val="50000"/>
-                    </a:prstClr>
-                  </a:innerShdw>
-                </a:effectLst>
-              </a14:hiddenEffects>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-            <a:prstTxWarp prst="textNoShape">
-              <a:avLst/>
-            </a:prstTxWarp>
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1000" b="0">
-                <a:solidFill>
-                  <a:srgbClr val="E8E8E8"/>
-                </a:solidFill>
-                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>Generate</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="17" name="Group 16">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2C760D2-7F54-4AC8-99E8-44A2F961B8EA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1732,18 +2472,18 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="5345390" y="733426"/>
-            <a:ext cx="612000" cy="1088687"/>
-            <a:chOff x="5168681" y="742951"/>
-            <a:chExt cx="612000" cy="1088687"/>
+            <a:off x="3803325" y="2381250"/>
+            <a:ext cx="1504950" cy="1440000"/>
+            <a:chOff x="6574150" y="2381250"/>
+            <a:chExt cx="1504950" cy="1440000"/>
           </a:xfrm>
         </xdr:grpSpPr>
-        <xdr:sp macro="[0]!ShtMain.BtnLvl1Click" textlink="">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="BtnLvl1">
+            <xdr:cNvPr id="33" name="Rectangle: Rounded Corners 32">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1751,8 +2491,131 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5168681" y="742951"/>
-              <a:ext cx="612000" cy="216000"/>
+              <a:off x="6574150" y="2381250"/>
+              <a:ext cx="1504950" cy="1440000"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst>
+                <a:gd name="adj" fmla="val 2500"/>
+              </a:avLst>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="6D6A75"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="35" name="Rectangle: Rounded Corners 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6574150" y="2381250"/>
+              <a:ext cx="1504950" cy="352425"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="DA2C38"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100">
+                  <a:solidFill>
+                    <a:srgbClr val="E8E8E8"/>
+                  </a:solidFill>
+                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Dependancy Report</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="[0]!ShtMain.BtnDepRepGenClick" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="36" name="BtnDepRepGen">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6810025" y="3074650"/>
+              <a:ext cx="1033200" cy="323850"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1815,28 +2678,55 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+              <a:prstTxWarp prst="textNoShape">
+                <a:avLst/>
+              </a:prstTxWarp>
+              <a:noAutofit/>
+            </a:bodyPr>
             <a:lstStyle/>
             <a:p>
-              <a:pPr algn="ctr"/>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1000" b="0">
                   <a:solidFill>
                     <a:srgbClr val="E8E8E8"/>
                   </a:solidFill>
                   <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>1</a:t>
+                <a:t>Generate</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnLvl2Click" textlink="">
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="57" name="Group 56">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0741997-08AA-4646-9389-33BCAA78ACCC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="5497825" y="2381250"/>
+            <a:ext cx="1504950" cy="1440000"/>
+            <a:chOff x="10307950" y="2381250"/>
+            <a:chExt cx="1504950" cy="1440000"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="BtnLvl2">
+            <xdr:cNvPr id="41" name="Rectangle: Rounded Corners 40">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2BF73BE-91C9-407D-8AC8-18B92DEA5BBB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1844,52 +2734,27 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5168681" y="962026"/>
-              <a:ext cx="612000" cy="216000"/>
+              <a:off x="10307950" y="2381250"/>
+              <a:ext cx="1504950" cy="1440000"/>
             </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
+            <a:prstGeom prst="roundRect">
+              <a:avLst>
+                <a:gd name="adj" fmla="val 2500"/>
+              </a:avLst>
             </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:srgbClr val="6D6A75"/>
+            </a:solidFill>
+            <a:ln>
               <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
           </xdr:spPr>
           <xdr:style>
             <a:lnRef idx="2">
@@ -1908,28 +2773,24 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>2</a:t>
-              </a:r>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </a:endParaRPr>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnLvl3Click" textlink="">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="BtnLvl3">
+            <xdr:cNvPr id="43" name="Rectangle: Rounded Corners 42">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52A39542-D204-47DE-942C-F3BEAD7DFE09}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1937,567 +2798,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5168681" y="1181101"/>
-              <a:ext cx="612000" cy="216000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>3</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnLvl4Click" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="BtnLvl4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5168681" y="1400176"/>
-              <a:ext cx="612000" cy="216000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>4</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnLvlAllClick" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="26" name="BtnLvlAll">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5168681" y="1615638"/>
-              <a:ext cx="612000" cy="216000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="DA2C38"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="DA2C38"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:effectLst>
-              <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                <a:prstClr val="black">
-                  <a:alpha val="50000"/>
-                </a:prstClr>
-              </a:innerShdw>
-            </a:effectLst>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="756A6D"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>All</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="23" name="TextBox 22">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5318015" y="495300"/>
-            <a:ext cx="666750" cy="209550"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="E8E8E8"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Level</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100"/>
-              <a:t> </a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="30" name="TextBox 29">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3231969" y="447676"/>
-            <a:ext cx="1454424" cy="276224"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="E8E8E8"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Look Ahead</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="E8E8E8"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> (wks)</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100"/>
-              <a:t> </a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="1025" name="TxtLAValue" hidden="1">
-                <a:extLst>
-                  <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                    <a14:compatExt spid="_x0000_s1025"/>
-                  </a:ext>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr bwMode="auto">
-              <a:xfrm>
-                <a:off x="3657600" y="733425"/>
-                <a:ext cx="609600" cy="266700"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:extLst>
-                <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                  <a14:hiddenLine w="9525">
-                    <a:noFill/>
-                    <a:miter lim="800000"/>
-                    <a:headEnd/>
-                    <a:tailEnd/>
-                  </a14:hiddenLine>
-                </a:ext>
-              </a:extLst>
-            </xdr:spPr>
-          </xdr:sp>
-        </mc:Choice>
-        <mc:Fallback/>
-      </mc:AlternateContent>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>603875</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>280025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>49575</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="18" name="Group 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="5414000" y="219075"/>
-          <a:ext cx="1504950" cy="1926000"/>
-          <a:chOff x="6572251" y="161925"/>
-          <a:chExt cx="1504950" cy="1926000"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6572251" y="161925"/>
-            <a:ext cx="1504950" cy="1926000"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 2500"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="6D6A75"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-GB" sz="1100">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="10" name="Group 9">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="6572251" y="161925"/>
-            <a:ext cx="1504950" cy="1660188"/>
-            <a:chOff x="6572251" y="161925"/>
-            <a:chExt cx="1504950" cy="1660188"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6572251" y="161925"/>
+              <a:off x="10307950" y="2381250"/>
               <a:ext cx="1504950" cy="352425"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
@@ -2530,25 +2831,30 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr algn="l"/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100">
                   <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
+                    <a:schemeClr val="lt1"/>
                   </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>Exception Report</a:t>
+                <a:t>Look Ahead Report</a:t>
               </a:r>
+              <a:endParaRPr lang="en-GB">
+                <a:effectLst/>
+              </a:endParaRPr>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnExcRepGenClick" textlink="">
+        <xdr:sp macro="[0]!ShtMain.BtnDepRepGenClick" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="37" name="BtnExcRepGen">
+            <xdr:cNvPr id="44" name="BtnDepRepGen">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{242CFAFE-E45C-49A7-86C7-973D985154C6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2556,7 +2862,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6808126" y="1498263"/>
+              <a:off x="10543825" y="3074650"/>
               <a:ext cx="1033200" cy="323850"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2649,23 +2955,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>30475</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>262870</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>59906</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>316225</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>49575</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>415270</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65644</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="32" name="Group 31">
+        <xdr:cNvPr id="61" name="Group 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B16A64C9-2324-4FB7-9399-787AA2E1C370}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2673,288 +2979,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7279000" y="219075"/>
-          <a:ext cx="1504950" cy="1926000"/>
-          <a:chOff x="6572251" y="161925"/>
-          <a:chExt cx="1504950" cy="1926000"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="33" name="Rectangle: Rounded Corners 32">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6572251" y="161925"/>
-            <a:ext cx="1504950" cy="1926000"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 2500"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="6D6A75"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-GB" sz="1100">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="34" name="Group 33">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="6572251" y="161925"/>
-            <a:ext cx="1504950" cy="1660188"/>
-            <a:chOff x="6572251" y="161925"/>
-            <a:chExt cx="1504950" cy="1660188"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="35" name="Rectangle: Rounded Corners 34">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6572251" y="161925"/>
-              <a:ext cx="1504950" cy="352425"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="DA2C38"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>Dependancy Report</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnDepRepGenClick" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="36" name="BtnDepRepGen">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6808126" y="1498263"/>
-              <a:ext cx="1033200" cy="323850"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-              <a:prstTxWarp prst="textNoShape">
-                <a:avLst/>
-              </a:prstTxWarp>
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" indent="0" algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>Generate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>62845</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>215245</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>5738</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="28" name="Group 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="672445" y="2657475"/>
-          <a:ext cx="762000" cy="967763"/>
-          <a:chOff x="659857" y="2657475"/>
-          <a:chExt cx="762000" cy="967763"/>
+          <a:off x="1482070" y="2345906"/>
+          <a:ext cx="762000" cy="958238"/>
+          <a:chOff x="672445" y="2686050"/>
+          <a:chExt cx="762000" cy="958238"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic macro="[0]!ThisWorkbook.ClearData">
@@ -2987,7 +3015,7 @@
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="659857" y="2657475"/>
+            <a:off x="672445" y="2686050"/>
             <a:ext cx="762000" cy="762000"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -3004,10 +3032,10 @@
       </xdr:pic>
       <xdr:sp macro="[0]!ThisWorkbook.ClearData" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="40" name="Rectangle: Rounded Corners 39">
+          <xdr:cNvPr id="62" name="Rectangle: Rounded Corners 61">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43333F61-A816-4877-900C-C565244CAA81}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3015,7 +3043,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="716857" y="3368063"/>
+            <a:off x="729445" y="3387113"/>
             <a:ext cx="648000" cy="257175"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -26092,7 +26120,7 @@
   <dimension ref="S3:U6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26139,7 +26167,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26152,16 +26179,16 @@
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>790575</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -26453,7 +26480,7 @@
     <col min="2" max="2" width="5.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.85546875" style="14" bestFit="1" customWidth="1"/>
@@ -26592,9 +26619,11 @@
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
       <c r="E7" s="17" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -26674,8 +26703,8 @@
   <cols>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="130.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -27363,7 +27392,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688A652D-6DD1-48EF-B210-1032D24E28CA}">
   <sheetPr codeName="ShtTaskView"/>
-  <dimension ref="C2:P205"/>
+  <dimension ref="C2:P227"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -29033,6 +29062,182 @@
         <v>30</v>
       </c>
     </row>
+    <row r="206" spans="4:14">
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="207" spans="4:14">
+      <c r="E207" t="s">
+        <v>19</v>
+      </c>
+      <c r="N207" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="208" spans="4:14">
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="209" spans="4:14">
+      <c r="E209" t="s">
+        <v>20</v>
+      </c>
+      <c r="N209" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="210" spans="4:14">
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="211" spans="4:14">
+      <c r="E211" t="s">
+        <v>21</v>
+      </c>
+      <c r="N211" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="212" spans="4:14">
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="213" spans="4:14">
+      <c r="E213" t="s">
+        <v>22</v>
+      </c>
+      <c r="N213" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="214" spans="4:14">
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="E214" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="215" spans="4:14">
+      <c r="E215" t="s">
+        <v>23</v>
+      </c>
+      <c r="N215" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="216" spans="4:14">
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="217" spans="4:14">
+      <c r="E217" t="s">
+        <v>24</v>
+      </c>
+      <c r="N217" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="218" spans="4:14">
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="219" spans="4:14">
+      <c r="E219" t="s">
+        <v>25</v>
+      </c>
+      <c r="N219" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="220" spans="4:14">
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="221" spans="4:14">
+      <c r="E221" t="s">
+        <v>26</v>
+      </c>
+      <c r="N221" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="222" spans="4:14">
+      <c r="D222">
+        <v>0</v>
+      </c>
+      <c r="E222" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="223" spans="4:14">
+      <c r="E223" t="s">
+        <v>27</v>
+      </c>
+      <c r="N223" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="224" spans="4:14">
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="225" spans="4:14">
+      <c r="E225" t="s">
+        <v>28</v>
+      </c>
+      <c r="N225" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="226" spans="4:14">
+      <c r="D226">
+        <v>0</v>
+      </c>
+      <c r="E226" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="227" spans="4:14">
+      <c r="E227" t="s">
+        <v>29</v>
+      </c>
+      <c r="N227" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C3:M2326">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
working on PPT export
</commit_message>
<xml_diff>
--- a/MSP Reporting Tool.xlsx
+++ b/MSP Reporting Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Development Areas\MSP Reporting Tool\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35A2718B-A59D-4712-89AE-18563521E19A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D707648F-771A-44BE-B6DF-6B9EF57CBA42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F7485911-4FC0-4026-A472-9F894C577CCD}"/>
   </bookViews>
@@ -16,15 +16,12 @@
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Dependancy Report" sheetId="248" r:id="rId2"/>
     <sheet name="Consolidated  Exception Report " sheetId="245" r:id="rId3"/>
-    <sheet name="Togo" sheetId="227" r:id="rId4"/>
-    <sheet name="Look Ahead Report (4)" sheetId="281" state="hidden" r:id="rId5"/>
-    <sheet name="Look Ahead Report (3)" sheetId="280" state="hidden" r:id="rId6"/>
-    <sheet name="Look Ahead Report (2)" sheetId="279" state="hidden" r:id="rId7"/>
-    <sheet name="Look Ahead Report" sheetId="246" state="hidden" r:id="rId8"/>
+    <sheet name="Plan Data" sheetId="227" r:id="rId4"/>
+    <sheet name="Look Ahead Report" sheetId="246" state="hidden" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_ff3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Data Sheets"}</definedName>
@@ -55,7 +52,7 @@
     <definedName name="xxxxxx" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Data Sheets"}</definedName>
     <definedName name="xxxxxx" hidden="1">{#N/A,#N/A,FALSE,"Data Sheets"}</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>DTI</t>
   </si>
@@ -135,103 +132,16 @@
     <t>Business Milestones</t>
   </si>
   <si>
-    <t>Donor</t>
-  </si>
-  <si>
-    <t>Local RAG</t>
-  </si>
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>got</t>
-  </si>
-  <si>
-    <t>Togo</t>
-  </si>
-  <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>Test Environment Strategy Complete</t>
-  </si>
-  <si>
-    <t>Solution Feasibility Report Signed Off</t>
-  </si>
-  <si>
-    <t>Group Compliance Checks Complete</t>
-  </si>
-  <si>
-    <t>CSOC Impact Assessment Complete</t>
-  </si>
-  <si>
-    <t>PSOC Impact Assessment Complete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Define Complete </t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>Design Start</t>
-  </si>
-  <si>
-    <t>Full Requirements Definition Signed Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mid Level Platform Designs Complete </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Test Phase&gt; Environment and Data Ready for Testing </t>
-  </si>
-  <si>
-    <t>Design Complete</t>
-  </si>
-  <si>
-    <t>Build Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build Complete </t>
-  </si>
-  <si>
-    <t>Test Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Acceptance Test Complete </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Functional Test Start </t>
-  </si>
-  <si>
-    <t>Non-Functional Test Complete</t>
-  </si>
-  <si>
-    <t>Test Complete</t>
-  </si>
-  <si>
-    <t>Develop Complete</t>
-  </si>
-  <si>
-    <t>Deploy Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deployment Start </t>
-  </si>
-  <si>
-    <t>Deployment Live</t>
-  </si>
-  <si>
     <t>C:\Users\Julian\OneDrive\Documents\OneSheet\titilayo ilesanmi\Planning template v3.1.mpp</t>
   </si>
   <si>
-    <t>20</t>
+    <t>1</t>
   </si>
   <si>
-    <t>AMBER</t>
+    <t>Exception Report</t>
+  </si>
+  <si>
+    <t>Look Ahead Report</t>
   </si>
 </sst>
 </file>
@@ -242,7 +152,7 @@
     <numFmt numFmtId="164" formatCode="dd\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,19 +185,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color indexed="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -305,8 +205,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,29 +253,146 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="18"/>
+        <fgColor rgb="FFF0935A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDA65"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -364,7 +401,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -376,47 +413,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,32 +430,20 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -466,6 +452,66 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,56 +539,80 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color theme="9" tint="0.39994506668294322"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right style="thin">
+          <color theme="9"/>
+        </right>
+        <top style="thin">
+          <color theme="9"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color theme="7" tint="0.39994506668294322"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+        <right style="thin">
+          <color theme="7"/>
+        </right>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
+        <color theme="5" tint="0.39994506668294322"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -644,6 +714,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFDA65"/>
+      <color rgb="FFFFDD71"/>
+      <color rgb="FFF0935A"/>
       <color rgb="FFDA2C38"/>
       <color rgb="FFE8E8E8"/>
       <color rgb="FF817E8A"/>
@@ -651,9 +724,6 @@
       <color rgb="FFBAC1B8"/>
       <color rgb="FF6D6A75"/>
       <color rgb="FF0F743C"/>
-      <color rgb="FFFC814A"/>
-      <color rgb="FF564256"/>
-      <color rgb="FFBFBFBF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1086,10 +1156,10 @@
                   <a:gradFill flip="none" rotWithShape="1">
                     <a:gsLst>
                       <a:gs pos="0">
-                        <a:srgbClr val="8A7E81"/>
+                        <a:srgbClr val="DA2C38"/>
                       </a:gs>
                       <a:gs pos="100000">
-                        <a:srgbClr val="8A7E81"/>
+                        <a:srgbClr val="DA2C38"/>
                       </a:gs>
                     </a:gsLst>
                     <a:lin ang="5400000" scaled="1"/>
@@ -1100,27 +1170,22 @@
                     <a:prstDash val="solid"/>
                     <a:miter lim="800000"/>
                   </a:ln>
-                  <a:effectLst/>
+                  <a:effectLst>
+                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                      <a:prstClr val="black">
+                        <a:alpha val="50000"/>
+                      </a:prstClr>
+                    </a:innerShdw>
+                  </a:effectLst>
                   <a:extLst>
                     <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                       <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
                         <a:solidFill>
-                          <a:srgbClr val="DA2C38"/>
+                          <a:srgbClr val="756A6D"/>
                         </a:solidFill>
                         <a:prstDash val="solid"/>
                         <a:miter lim="800000"/>
                       </a14:hiddenLine>
-                    </a:ext>
-                    <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                      <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                        <a:effectLst>
-                          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                            <a:prstClr val="black">
-                              <a:alpha val="50000"/>
-                            </a:prstClr>
-                          </a:innerShdw>
-                        </a:effectLst>
-                      </a14:hiddenEffects>
                     </a:ext>
                   </a:extLst>
                 </xdr:spPr>
@@ -1458,10 +1523,10 @@
                   <a:gradFill flip="none" rotWithShape="1">
                     <a:gsLst>
                       <a:gs pos="0">
-                        <a:srgbClr val="DA2C38"/>
+                        <a:srgbClr val="8A7E81"/>
                       </a:gs>
                       <a:gs pos="100000">
-                        <a:srgbClr val="DA2C38"/>
+                        <a:srgbClr val="8A7E81"/>
                       </a:gs>
                     </a:gsLst>
                     <a:lin ang="5400000" scaled="1"/>
@@ -1472,22 +1537,27 @@
                     <a:prstDash val="solid"/>
                     <a:miter lim="800000"/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                   <a:extLst>
                     <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                       <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
                         <a:solidFill>
-                          <a:srgbClr val="756A6D"/>
+                          <a:srgbClr val="DA2C38"/>
                         </a:solidFill>
                         <a:prstDash val="solid"/>
                         <a:miter lim="800000"/>
                       </a14:hiddenLine>
+                    </a:ext>
+                    <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                      <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                        <a:effectLst>
+                          <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                            <a:prstClr val="black">
+                              <a:alpha val="50000"/>
+                            </a:prstClr>
+                          </a:innerShdw>
+                        </a:effectLst>
+                      </a14:hiddenEffects>
                     </a:ext>
                   </a:extLst>
                 </xdr:spPr>
@@ -1726,17 +1796,96 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>321950</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>116025</xdr:rowOff>
     </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676525" y="2105025"/>
+          <a:ext cx="1504950" cy="1440000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 2500"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="6D6A75"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>474000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>188575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>354675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>110575</xdr:rowOff>
+    </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="1024" name="Group 1023">
+        <xdr:cNvPr id="24" name="Group 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000000040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6DF9EEA-9995-48CE-8125-C5536EEB5E33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1744,747 +1893,533 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2676525" y="2105025"/>
-          <a:ext cx="4893950" cy="1440000"/>
-          <a:chOff x="2108825" y="2381250"/>
-          <a:chExt cx="4893950" cy="1440000"/>
+          <a:off x="2912400" y="2665075"/>
+          <a:ext cx="1033200" cy="684000"/>
+          <a:chOff x="2912400" y="2569825"/>
+          <a:chExt cx="1033200" cy="684000"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="55" name="Group 54">
+      <xdr:sp macro="[0]!ShtMain.BtnExcRepGenClick" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="BtnExcRepGen">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
           <a:xfrm>
-            <a:off x="2108825" y="2381250"/>
-            <a:ext cx="1504950" cy="1440000"/>
-            <a:chOff x="2032625" y="2381250"/>
-            <a:chExt cx="1504950" cy="1440000"/>
+            <a:off x="2912400" y="2569825"/>
+            <a:ext cx="1033200" cy="684000"/>
           </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2032625" y="2381250"/>
-              <a:ext cx="1504950" cy="1440000"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 2500"/>
-              </a:avLst>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="6D6A75"/>
-            </a:solidFill>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+            <a:tileRect/>
+          </a:gradFill>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="800000"/>
+          </a:ln>
+          <a:effectLst/>
+          <a:extLst>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="DA2C38"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a14:hiddenLine>
+            </a:ext>
+            <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+              <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:effectLst>
+                  <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                    <a:prstClr val="black">
+                      <a:alpha val="50000"/>
+                    </a:prstClr>
+                  </a:innerShdw>
+                </a:effectLst>
+              </a14:hiddenEffects>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:endParaRPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="E8E8E8"/>
+              </a:solidFill>
+              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="17" name="Graphic 16" descr="Warning">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F281A97-B239-4CFD-B24F-DFC7B5A8B5CC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3159000" y="2641825"/>
+            <a:ext cx="540000" cy="540000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676525" y="2105025"/>
+          <a:ext cx="1504950" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DA2C38"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="E8E8E8"/>
+              </a:solidFill>
+              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Exception Report</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>170500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>456250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle: Rounded Corners 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4371025" y="2105025"/>
+          <a:ext cx="1504950" cy="1440000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 2500"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="6D6A75"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100">
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-GB" sz="1100">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2032625" y="2381250"/>
-              <a:ext cx="1504950" cy="352425"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="DA2C38"/>
-            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>170500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>456250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rectangle: Rounded Corners 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4371025" y="2105025"/>
+          <a:ext cx="1504950" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DA2C38"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="E8E8E8"/>
+              </a:solidFill>
+              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Dependancy Report</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>36200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>321950</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Rectangle: Rounded Corners 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6065525" y="2105025"/>
+          <a:ext cx="1504950" cy="1440000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 2500"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="6D6A75"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100">
             <a:ln>
               <a:noFill/>
             </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>Exception Report</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnExcRepGenClick" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="37" name="BtnExcRepGen">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2268500" y="3074650"/>
-              <a:ext cx="1033200" cy="323850"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>36200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>321950</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Rectangle: Rounded Corners 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6065525" y="2105025"/>
+          <a:ext cx="1504950" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DA2C38"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Look Ahead Report</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
             <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-              <a:prstTxWarp prst="textNoShape">
-                <a:avLst/>
-              </a:prstTxWarp>
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" indent="0" algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>Generate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="56" name="Group 55">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="3803325" y="2381250"/>
-            <a:ext cx="1504950" cy="1440000"/>
-            <a:chOff x="6574150" y="2381250"/>
-            <a:chExt cx="1504950" cy="1440000"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="33" name="Rectangle: Rounded Corners 32">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6574150" y="2381250"/>
-              <a:ext cx="1504950" cy="1440000"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 2500"/>
-              </a:avLst>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="6D6A75"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-GB" sz="1100">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="35" name="Rectangle: Rounded Corners 34">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6574150" y="2381250"/>
-              <a:ext cx="1504950" cy="352425"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="DA2C38"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                </a:rPr>
-                <a:t>Dependancy Report</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnDepRepGenClick" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="36" name="BtnDepRepGen">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6810025" y="3074650"/>
-              <a:ext cx="1033200" cy="323850"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-              <a:prstTxWarp prst="textNoShape">
-                <a:avLst/>
-              </a:prstTxWarp>
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" indent="0" algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>Generate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="57" name="Group 56">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="5497825" y="2381250"/>
-            <a:ext cx="1504950" cy="1440000"/>
-            <a:chOff x="10307950" y="2381250"/>
-            <a:chExt cx="1504950" cy="1440000"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="41" name="Rectangle: Rounded Corners 40">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10307950" y="2381250"/>
-              <a:ext cx="1504950" cy="1440000"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 2500"/>
-              </a:avLst>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="6D6A75"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-GB" sz="1100">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="43" name="Rectangle: Rounded Corners 42">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10307950" y="2381250"/>
-              <a:ext cx="1504950" cy="352425"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="DA2C38"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>Look Ahead Report</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-GB">
-                <a:effectLst/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="[0]!ShtMain.BtnLARGenClick" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="44" name="BtnLARGen">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10543825" y="3074650"/>
-              <a:ext cx="1033200" cy="323850"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="8A7E81"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="DA2C38"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
-                      <a:prstClr val="black">
-                        <a:alpha val="50000"/>
-                      </a:prstClr>
-                    </a:innerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-              <a:prstTxWarp prst="textNoShape">
-                <a:avLst/>
-              </a:prstTxWarp>
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" indent="0" algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0">
-                  <a:solidFill>
-                    <a:srgbClr val="E8E8E8"/>
-                  </a:solidFill>
-                  <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>Generate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-    </xdr:grpSp>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -2533,13 +2468,13 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
               </a:ext>
               <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId5"/>
               </a:ext>
             </a:extLst>
           </a:blip>
@@ -2764,7 +2699,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2794,6 +2729,346 @@
               </a14:hiddenFill>
             </a:ext>
           </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>188575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>220375</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>110575</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="Group 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3988A4AA-5366-461F-A653-AFEB5A25FFD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4606900" y="2665075"/>
+          <a:ext cx="1033200" cy="684000"/>
+          <a:chOff x="4606900" y="2798425"/>
+          <a:chExt cx="1033200" cy="684000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="[0]!ShtMain.BtnDepRepGenClick" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="BtnDepRepGen">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4606900" y="2798425"/>
+            <a:ext cx="1033200" cy="684000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+            <a:tileRect/>
+          </a:gradFill>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="800000"/>
+          </a:ln>
+          <a:effectLst/>
+          <a:extLst>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="DA2C38"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a14:hiddenLine>
+            </a:ext>
+            <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+              <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:effectLst>
+                  <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                    <a:prstClr val="black">
+                      <a:alpha val="50000"/>
+                    </a:prstClr>
+                  </a:innerShdw>
+                </a:effectLst>
+              </a14:hiddenEffects>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:endParaRPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="E8E8E8"/>
+              </a:solidFill>
+              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic macro="[0]!ShtMain.BtnDepRepGenClick">
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="Graphic 8" descr="Link">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5EEBC32-A5BC-41C8-BE94-7231FAD9644A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4853500" y="2870425"/>
+            <a:ext cx="540000" cy="540000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>272075</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>188575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>86075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>110575</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Group 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A38CCB-5140-4ACE-ADD2-09E8887E0153}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6301400" y="2665075"/>
+          <a:ext cx="1033200" cy="684000"/>
+          <a:chOff x="6301400" y="2798425"/>
+          <a:chExt cx="1033200" cy="684000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="[0]!ShtMain.BtnLARGenClick" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="BtnLARGen">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6301400" y="2798425"/>
+            <a:ext cx="1033200" cy="684000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:srgbClr val="8A7E81"/>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+            <a:tileRect/>
+          </a:gradFill>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="800000"/>
+          </a:ln>
+          <a:effectLst/>
+          <a:extLst>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="DA2C38"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a14:hiddenLine>
+            </a:ext>
+            <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+              <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:effectLst>
+                  <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                    <a:prstClr val="black">
+                      <a:alpha val="50000"/>
+                    </a:prstClr>
+                  </a:innerShdw>
+                </a:effectLst>
+              </a14:hiddenEffects>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:endParaRPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="E8E8E8"/>
+              </a:solidFill>
+              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic macro="[0]!ShtMain.BtnLARGenClick">
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="11" name="Graphic 10" descr="Diamond Suit">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD89EF34-B55E-4080-821A-C80845302DD3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId10"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6548000" y="2870425"/>
+            <a:ext cx="540000" cy="540000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
         </xdr:spPr>
       </xdr:pic>
     </xdr:grpSp>
@@ -25814,7 +26089,7 @@
   <dimension ref="S3:U6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25823,50 +26098,41 @@
     <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="17" width="9.140625" style="3"/>
     <col min="18" max="18" width="16.85546875" style="3" customWidth="1"/>
-    <col min="19" max="21" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="16.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="16.85546875" style="3" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="19:21">
+    <row r="3" spans="19:20">
       <c r="S3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="T3" s="4">
-        <v>3</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="19:21">
+    <row r="4" spans="19:20">
       <c r="S4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="19:21">
+    <row r="5" spans="19:20">
       <c r="S5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="T5" s="4">
-        <v>9999</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="19:21">
+    <row r="6" spans="19:20">
       <c r="S6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -25911,817 +26177,207 @@
   <sheetPr codeName="ShtDepLog">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:W24"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="26.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="24"/>
-    <col min="2" max="2" width="4.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="27" customWidth="1"/>
-    <col min="8" max="8" width="9" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="26" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="26"/>
-    <col min="14" max="14" width="9.5703125" style="27"/>
-    <col min="15" max="16" width="9.5703125" style="28"/>
-    <col min="17" max="17" width="9.5703125" style="29"/>
-    <col min="18" max="20" width="9.5703125" style="28"/>
-    <col min="21" max="23" width="9.5703125" style="25"/>
+    <col min="1" max="1" width="9.5703125" style="11"/>
+    <col min="2" max="2" width="4" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="14"/>
+    <col min="15" max="16" width="9.5703125" style="15"/>
+    <col min="17" max="17" width="9.5703125" style="16"/>
+    <col min="18" max="20" width="9.5703125" style="15"/>
+    <col min="21" max="23" width="9.5703125" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B2" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>18</v>
-      </c>
+    <row r="1" spans="1:16" ht="26.25" customHeight="1">
+      <c r="A1" s="41"/>
     </row>
-    <row r="3" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B3" s="24">
-        <v>79</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="25">
-        <v>5</v>
-      </c>
-      <c r="E3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="37">
-        <v>44044</v>
-      </c>
-      <c r="J3" s="37">
-        <v>43966</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" s="28" t="s">
-        <v>23</v>
-      </c>
+    <row r="2" spans="1:16" ht="26.25" customHeight="1">
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
     </row>
-    <row r="4" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B4" s="24">
-        <v>6</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="25">
-        <v>5</v>
-      </c>
-      <c r="E4" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="37">
-        <v>44044</v>
-      </c>
-      <c r="J4" s="37">
-        <v>46227</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="28" t="s">
-        <v>23</v>
-      </c>
+    <row r="3" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
     </row>
-    <row r="5" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B5" s="24">
-        <v>7</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="25">
-        <v>5</v>
-      </c>
-      <c r="E5" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="37">
-        <v>44044</v>
-      </c>
-      <c r="J5" s="37">
-        <v>46227</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="28" t="s">
-        <v>23</v>
-      </c>
+    <row r="4" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
-    <row r="6" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B6" s="24">
-        <v>8</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="25">
-        <v>5</v>
-      </c>
-      <c r="E6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="37">
-        <v>44044</v>
-      </c>
-      <c r="J6" s="37">
-        <v>43966</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="28" t="s">
-        <v>23</v>
-      </c>
+    <row r="5" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
-    <row r="7" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B7" s="24">
-        <v>9</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="25">
-        <v>5</v>
-      </c>
-      <c r="E7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="37">
-        <v>44044</v>
-      </c>
-      <c r="J7" s="37">
-        <v>46227</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="28" t="s">
-        <v>23</v>
-      </c>
+    <row r="6" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
     </row>
-    <row r="8" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B8" s="24">
-        <v>11</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="25">
-        <v>5</v>
-      </c>
-      <c r="E8" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="37">
-        <v>44044</v>
-      </c>
-      <c r="J8" s="37">
-        <v>43966</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="28" t="s">
-        <v>24</v>
-      </c>
+    <row r="7" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
-    <row r="9" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B9" s="24">
-        <v>13</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="25">
-        <v>11</v>
-      </c>
-      <c r="E9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J9" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="28" t="s">
-        <v>24</v>
-      </c>
+    <row r="8" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
     </row>
-    <row r="10" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B10" s="24">
-        <v>14</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="25">
-        <v>11</v>
-      </c>
-      <c r="E10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J10" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="28" t="s">
-        <v>24</v>
-      </c>
+    <row r="9" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
     </row>
-    <row r="11" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B11" s="24">
-        <v>81</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="25">
-        <v>11</v>
-      </c>
-      <c r="E11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J11" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="28" t="s">
-        <v>24</v>
-      </c>
+    <row r="10" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
-    <row r="12" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B12" s="24">
-        <v>82</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="25">
-        <v>11</v>
-      </c>
-      <c r="E12" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J12" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="28" t="s">
-        <v>24</v>
-      </c>
+    <row r="11" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
-    <row r="13" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B13" s="24">
-        <v>15</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="25">
-        <v>11</v>
-      </c>
-      <c r="E13" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J13" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" s="28" t="s">
-        <v>24</v>
-      </c>
+    <row r="12" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
     </row>
-    <row r="14" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B14" s="24">
-        <v>16</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="25">
-        <v>11</v>
-      </c>
-      <c r="E14" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J14" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P14" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="13" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
     </row>
-    <row r="15" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B15" s="24">
-        <v>17</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="25">
-        <v>11</v>
-      </c>
-      <c r="E15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J15" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="14" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
-    <row r="16" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B16" s="24">
-        <v>18</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="25">
-        <v>11</v>
-      </c>
-      <c r="E16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J16" s="37">
-        <v>43987</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P16" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="15" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
-    <row r="17" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B17" s="24">
-        <v>86</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="25">
-        <v>10</v>
-      </c>
-      <c r="E17" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J17" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="16" spans="1:16" ht="26.25" customHeight="1">
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
-    <row r="18" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B18" s="24">
-        <v>84</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="25">
-        <v>10</v>
-      </c>
-      <c r="E18" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J18" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P18" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="17" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
     </row>
-    <row r="19" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B19" s="24">
-        <v>83</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="25">
-        <v>10</v>
-      </c>
-      <c r="E19" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J19" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L19" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P19" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="18" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
-    <row r="20" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B20" s="24">
-        <v>19</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="25">
-        <v>10</v>
-      </c>
-      <c r="E20" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J20" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P20" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="19" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
-    <row r="21" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B21" s="24">
-        <v>20</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="25">
-        <v>10</v>
-      </c>
-      <c r="E21" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J21" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K21" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P21" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="20" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
-    <row r="22" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B22" s="24">
-        <v>21</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="25">
-        <v>10</v>
-      </c>
-      <c r="E22" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J22" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K22" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L22" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P22" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="21" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
     </row>
-    <row r="23" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B23" s="24">
-        <v>22</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="25">
-        <v>10</v>
-      </c>
-      <c r="E23" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="37">
-        <v>43952</v>
-      </c>
-      <c r="J23" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K23" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L23" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P23" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="22" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
-    <row r="24" spans="2:16" ht="26.25" customHeight="1">
-      <c r="B24" s="24">
-        <v>23</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="25">
-        <v>10</v>
-      </c>
-      <c r="E24" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="37">
-        <v>43959</v>
-      </c>
-      <c r="J24" s="37">
-        <v>44002</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L24" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P24" s="28" t="s">
-        <v>25</v>
-      </c>
+    <row r="23" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" spans="9:10" ht="26.25" customHeight="1">
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"Aligned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"Donor BL earlier than Beneficiary"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
       <formula>"Alignment Issue"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576 G1:G1048576">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"AMBER"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"RED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"COMPLETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>"GREEN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"COMPLETE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:F1048576">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:L1 K3:L1048576">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>K1="RED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>K1="AMBER"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>K1="GREEN"</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.3" right="0.17" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="64" orientation="landscape" r:id="rId1"/>
@@ -26733,94 +26389,83 @@
   <sheetPr codeName="ShtExceptRep"/>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="24" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:12" ht="26.25">
+      <c r="A1" s="41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="21" customHeight="1">
-      <c r="A2" s="31"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="8"/>
-    </row>
     <row r="3" spans="1:12" ht="20.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4"/>
@@ -26837,23 +26482,23 @@
       <c r="L4"/>
     </row>
     <row r="5" spans="1:12" ht="20.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="33"/>
+      <c r="A6" s="18"/>
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6" s="6"/>
@@ -26867,20 +26512,20 @@
       <c r="L6"/>
     </row>
     <row r="7" spans="1:12" ht="20.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="40"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8"/>
@@ -26897,20 +26542,20 @@
       <c r="L8"/>
     </row>
     <row r="9" spans="1:12" ht="20.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10"/>
@@ -26934,10 +26579,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A9EE8F-EDC6-401D-AECC-57882115D77B}">
   <sheetPr codeName="ShtPlanData"/>
-  <dimension ref="C1:N136"/>
+  <dimension ref="E3:N136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26956,110 +26601,70 @@
     <col min="14" max="14" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:14">
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="3:14">
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="3:14">
+    <row r="3" spans="5:7">
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="3:14">
+    <row r="4" spans="5:7">
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="3:14">
+    <row r="5" spans="5:7">
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="3:14">
+    <row r="6" spans="5:7">
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="3:14">
+    <row r="7" spans="5:7">
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="3:14">
+    <row r="8" spans="5:7">
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="3:14">
+    <row r="9" spans="5:7">
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="3:14">
+    <row r="10" spans="5:7">
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="3:14">
+    <row r="11" spans="5:7">
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="3:14">
+    <row r="12" spans="5:7">
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="3:14">
+    <row r="13" spans="5:7">
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="3:14">
+    <row r="14" spans="5:7">
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="3:14">
+    <row r="15" spans="5:7">
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="3:14">
+    <row r="16" spans="5:7">
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -27670,12 +27275,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B747CF41-4668-4D03-A3C8-B4F1B5EA35DD}">
-  <sheetPr codeName="ShtTaskView3"/>
-  <dimension ref="C2:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688A652D-6DD1-48EF-B210-1032D24E28CA}">
+  <sheetPr codeName="ShtTaskView"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15"/>
@@ -27684,150 +27289,17 @@
     <col min="2" max="2" width="5.140625" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.85546875" style="22"/>
-    <col min="8" max="8" width="15.85546875" style="23"/>
-    <col min="9" max="13" width="15.85546875" style="22"/>
+    <col min="6" max="7" width="15.85546875" style="9"/>
+    <col min="8" max="8" width="15.85546875" style="10"/>
+    <col min="9" max="13" width="15.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" s="21" customFormat="1">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
+    <row r="1" spans="1:13" ht="26.25">
+      <c r="A1" s="41" t="s">
+        <v>23</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
     </row>
-  </sheetData>
-  <conditionalFormatting sqref="C3:M2101">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>AND($D3="", $E3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14F96C8-8CA8-4A13-B7DE-B3C8739B31AA}">
-  <sheetPr codeName="ShtTaskView2"/>
-  <dimension ref="C2:M2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.85546875" style="22"/>
-    <col min="8" max="8" width="15.85546875" style="23"/>
-    <col min="9" max="13" width="15.85546875" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:13" s="21" customFormat="1">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C3:M2101">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>AND($D3="", $E3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734983D7-9A66-45CE-9374-CB12B0F93866}">
-  <sheetPr codeName="ShtTaskView1"/>
-  <dimension ref="C2:M2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.85546875" style="22"/>
-    <col min="8" max="8" width="15.85546875" style="23"/>
-    <col min="9" max="13" width="15.85546875" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:13" s="21" customFormat="1">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C3:M2101">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND($D3="", $E3&lt;&gt;"")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688A652D-6DD1-48EF-B210-1032D24E28CA}">
-  <sheetPr codeName="ShtTaskView"/>
-  <dimension ref="C2:M2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.85546875" style="22"/>
-    <col min="8" max="8" width="15.85546875" style="23"/>
-    <col min="9" max="13" width="15.85546875" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:13" s="21" customFormat="1">
+    <row r="2" spans="1:13" s="8" customFormat="1">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">

</xml_diff>